<commit_message>
Update modbus poll workspace.
</commit_message>
<xml_diff>
--- a/通讯协议.xlsx
+++ b/通讯协议.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\Irixi\006 4x25G DML TOSA\Fanout Board\Firmware\4x25G_DML_TOSA_PowerSupply\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\Irixi\006 4x25G DML TOSA\Power Supply Board\Firmware\4x25G_DML_TOSA_PowerSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134517C0-69C2-4B53-98E6-5430048AE3E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1AEE69-07CF-44E5-A985-EB8388239B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Error Code" sheetId="2" r:id="rId2"/>
+    <sheet name="配置参数" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="207">
   <si>
     <t>Colis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -758,6 +759,138 @@
 0：禁用Tx
 1：使能Tx</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Op Mode 1</t>
+  </si>
+  <si>
+    <t>VSHCT 1</t>
+  </si>
+  <si>
+    <t>VBUSCT 1</t>
+  </si>
+  <si>
+    <t>Avg Mode 1</t>
+  </si>
+  <si>
+    <t>Max Current 1</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Shunt Res Ohm 1</t>
+  </si>
+  <si>
+    <t>Op Mode 2</t>
+  </si>
+  <si>
+    <t>VSHCT 2</t>
+  </si>
+  <si>
+    <t>VBUSCT 2</t>
+  </si>
+  <si>
+    <t>Avg Mode 2</t>
+  </si>
+  <si>
+    <t>Max Current 2</t>
+  </si>
+  <si>
+    <t>Shunt Res Ohm 2</t>
+  </si>
+  <si>
+    <t>Op Mode 3</t>
+  </si>
+  <si>
+    <t>VSHCT 3</t>
+  </si>
+  <si>
+    <t>VBUSCT 3</t>
+  </si>
+  <si>
+    <t>Avg Mode 3</t>
+  </si>
+  <si>
+    <t>Max Current 3</t>
+  </si>
+  <si>
+    <t>Shunt Res Ohm 3</t>
+  </si>
+  <si>
+    <t>Op Mode 24V</t>
+  </si>
+  <si>
+    <t>VSHCT 24V</t>
+  </si>
+  <si>
+    <t>VBUSCT 24V</t>
+  </si>
+  <si>
+    <t>Avg Mode 24V</t>
+  </si>
+  <si>
+    <t>Max Current 24V</t>
+  </si>
+  <si>
+    <t>Shunt Res Ohm 24V</t>
+  </si>
+  <si>
+    <t>Op Mode TEC</t>
+  </si>
+  <si>
+    <t>VBUSCT TEC</t>
+  </si>
+  <si>
+    <t>Avg Mode TEC</t>
+  </si>
+  <si>
+    <t>Max Current TEC</t>
+  </si>
+  <si>
+    <t>Shunt Res Ohm TEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0000 0000 0000 0011 </t>
+  </si>
+  <si>
+    <t>PID kp</t>
+  </si>
+  <si>
+    <t>PID ki</t>
+  </si>
+  <si>
+    <t>PID kd</t>
+  </si>
+  <si>
+    <t>Sampling Interval(ms)</t>
+  </si>
+  <si>
+    <t>NTC Coeff A</t>
+  </si>
+  <si>
+    <t>NTC Coeff B</t>
+  </si>
+  <si>
+    <t>NTC Coeff C</t>
+  </si>
+  <si>
+    <t>NTC Ref. Resistor(ohm)</t>
+  </si>
+  <si>
+    <t>Vref NTC (V)</t>
+  </si>
+  <si>
+    <t>Vref MCU (V)</t>
+  </si>
+  <si>
+    <t>Temp. Protection Low</t>
+  </si>
+  <si>
+    <t>Temp. Protection High</t>
+  </si>
+  <si>
+    <t>Target Temp (C)</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1134,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1100,72 +1233,73 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1672,7 +1806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A76" workbookViewId="0">
       <selection activeCell="J7" sqref="J7:J8"/>
     </sheetView>
   </sheetViews>
@@ -1695,24 +1829,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47" t="s">
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
@@ -1759,7 +1893,7 @@
       <c r="B3" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="47" t="s">
         <v>133</v>
       </c>
       <c r="D3" s="28" t="s">
@@ -1768,13 +1902,13 @@
       <c r="E3" s="18">
         <v>0</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="55" t="s">
+      <c r="G3" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="H3" s="52" t="s">
+      <c r="H3" s="43" t="s">
         <v>83</v>
       </c>
       <c r="I3" s="18">
@@ -1797,16 +1931,16 @@
       <c r="B4" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="48"/>
       <c r="D4" s="29" t="s">
         <v>85</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="48"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="36"/>
       <c r="I4" s="10">
         <v>1</v>
       </c>
@@ -1827,20 +1961,20 @@
       <c r="B5" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="51"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="29" t="s">
         <v>85</v>
       </c>
       <c r="E5" s="10">
         <v>2</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="48" t="s">
+      <c r="H5" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I5" s="10">
@@ -1872,9 +2006,9 @@
       <c r="E6" s="10">
         <v>3</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="48"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="36"/>
       <c r="I6" s="10">
         <v>3</v>
       </c>
@@ -1904,25 +2038,25 @@
       <c r="E7" s="10">
         <v>4</v>
       </c>
-      <c r="F7" s="49" t="s">
+      <c r="F7" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I7" s="10">
         <v>4</v>
       </c>
-      <c r="J7" s="44" t="s">
+      <c r="J7" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="K7" s="40" t="s">
+      <c r="K7" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1942,15 +2076,15 @@
       <c r="E8" s="10">
         <v>5</v>
       </c>
-      <c r="F8" s="49"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="48"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="36"/>
       <c r="I8" s="10">
         <v>5</v>
       </c>
-      <c r="J8" s="44"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="39"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="51"/>
     </row>
     <row r="9" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
@@ -1968,25 +2102,25 @@
       <c r="E9" s="10">
         <v>6</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="48" t="s">
+      <c r="H9" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I9" s="10">
         <v>6</v>
       </c>
-      <c r="J9" s="44" t="s">
+      <c r="J9" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="50" t="s">
         <v>90</v>
       </c>
-      <c r="L9" s="39" t="s">
+      <c r="L9" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1998,15 +2132,15 @@
       <c r="E10" s="10">
         <v>7</v>
       </c>
-      <c r="F10" s="49"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="48"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="36"/>
       <c r="I10" s="10">
         <v>7</v>
       </c>
-      <c r="J10" s="44"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="39"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="51"/>
     </row>
     <row r="11" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
@@ -2016,13 +2150,13 @@
       <c r="E11" s="10">
         <v>8</v>
       </c>
-      <c r="F11" s="49" t="s">
+      <c r="F11" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I11" s="10">
@@ -2031,7 +2165,7 @@
       <c r="J11" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="38" t="s">
         <v>97</v>
       </c>
       <c r="L11" s="32" t="s">
@@ -2046,16 +2180,16 @@
       <c r="E12" s="10">
         <v>9</v>
       </c>
-      <c r="F12" s="49"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="48"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="10">
         <v>9</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="K12" s="36"/>
+      <c r="K12" s="38"/>
       <c r="L12" s="32" t="s">
         <v>86</v>
       </c>
@@ -2068,11 +2202,11 @@
       <c r="E13" s="10">
         <v>10</v>
       </c>
-      <c r="F13" s="49" t="s">
+      <c r="F13" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="36"/>
-      <c r="H13" s="48" t="s">
+      <c r="G13" s="38"/>
+      <c r="H13" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I13" s="10">
@@ -2081,7 +2215,7 @@
       <c r="J13" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="K13" s="36"/>
+      <c r="K13" s="38"/>
       <c r="L13" s="32" t="s">
         <v>86</v>
       </c>
@@ -2094,16 +2228,16 @@
       <c r="E14" s="10">
         <v>11</v>
       </c>
-      <c r="F14" s="49"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="48"/>
+      <c r="F14" s="37"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="36"/>
       <c r="I14" s="10">
         <v>11</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="K14" s="36"/>
+      <c r="K14" s="38"/>
       <c r="L14" s="32" t="s">
         <v>86</v>
       </c>
@@ -2116,21 +2250,21 @@
       <c r="E15" s="10">
         <v>12</v>
       </c>
-      <c r="F15" s="49" t="s">
+      <c r="F15" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="36"/>
-      <c r="H15" s="48" t="s">
+      <c r="G15" s="38"/>
+      <c r="H15" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I15" s="10">
         <v>12</v>
       </c>
-      <c r="J15" s="44" t="s">
+      <c r="J15" s="46" t="s">
         <v>96</v>
       </c>
-      <c r="K15" s="36"/>
-      <c r="L15" s="39" t="s">
+      <c r="K15" s="38"/>
+      <c r="L15" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2142,15 +2276,15 @@
       <c r="E16" s="10">
         <v>13</v>
       </c>
-      <c r="F16" s="49"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="48"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="36"/>
       <c r="I16" s="10">
         <v>13</v>
       </c>
-      <c r="J16" s="44"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="39"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="51"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
@@ -2160,21 +2294,21 @@
       <c r="E17" s="10">
         <v>14</v>
       </c>
-      <c r="F17" s="49" t="s">
+      <c r="F17" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="48" t="s">
+      <c r="G17" s="38"/>
+      <c r="H17" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I17" s="10">
         <v>14</v>
       </c>
-      <c r="J17" s="44" t="s">
+      <c r="J17" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="K17" s="36"/>
-      <c r="L17" s="39" t="s">
+      <c r="K17" s="38"/>
+      <c r="L17" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2186,15 +2320,15 @@
       <c r="E18" s="10">
         <v>15</v>
       </c>
-      <c r="F18" s="49"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="48"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="36"/>
       <c r="I18" s="10">
         <v>15</v>
       </c>
-      <c r="J18" s="44"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="39"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="51"/>
     </row>
     <row r="19" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
@@ -2204,13 +2338,13 @@
       <c r="E19" s="10">
         <v>16</v>
       </c>
-      <c r="F19" s="49" t="s">
+      <c r="F19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="36" t="s">
+      <c r="G19" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I19" s="10">
@@ -2219,7 +2353,7 @@
       <c r="J19" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="K19" s="36" t="s">
+      <c r="K19" s="38" t="s">
         <v>159</v>
       </c>
       <c r="L19" s="32" t="s">
@@ -2234,16 +2368,16 @@
       <c r="E20" s="10">
         <v>17</v>
       </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="48"/>
+      <c r="F20" s="37"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="36"/>
       <c r="I20" s="10">
         <v>17</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="K20" s="36"/>
+      <c r="K20" s="38"/>
       <c r="L20" s="32" t="s">
         <v>86</v>
       </c>
@@ -2256,11 +2390,11 @@
       <c r="E21" s="10">
         <v>18</v>
       </c>
-      <c r="F21" s="49" t="s">
+      <c r="F21" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="36"/>
-      <c r="H21" s="48" t="s">
+      <c r="G21" s="38"/>
+      <c r="H21" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I21" s="10">
@@ -2269,7 +2403,7 @@
       <c r="J21" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="36"/>
+      <c r="K21" s="38"/>
       <c r="L21" s="32" t="s">
         <v>86</v>
       </c>
@@ -2282,16 +2416,16 @@
       <c r="E22" s="10">
         <v>19</v>
       </c>
-      <c r="F22" s="49"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="48"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="36"/>
       <c r="I22" s="10">
         <v>19</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="36"/>
+      <c r="K22" s="38"/>
       <c r="L22" s="32" t="s">
         <v>86</v>
       </c>
@@ -2304,21 +2438,21 @@
       <c r="E23" s="10">
         <v>20</v>
       </c>
-      <c r="F23" s="49" t="s">
+      <c r="F23" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="G23" s="36"/>
-      <c r="H23" s="48" t="s">
+      <c r="G23" s="38"/>
+      <c r="H23" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I23" s="10">
         <v>20</v>
       </c>
-      <c r="J23" s="44" t="s">
+      <c r="J23" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="K23" s="36"/>
-      <c r="L23" s="39" t="s">
+      <c r="K23" s="38"/>
+      <c r="L23" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2330,15 +2464,15 @@
       <c r="E24" s="10">
         <v>21</v>
       </c>
-      <c r="F24" s="49"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="48"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="36"/>
       <c r="I24" s="10">
         <v>21</v>
       </c>
-      <c r="J24" s="44"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="39"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="51"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
@@ -2348,21 +2482,21 @@
       <c r="E25" s="10">
         <v>22</v>
       </c>
-      <c r="F25" s="49" t="s">
+      <c r="F25" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="36"/>
-      <c r="H25" s="48" t="s">
+      <c r="G25" s="38"/>
+      <c r="H25" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I25" s="10">
         <v>22</v>
       </c>
-      <c r="J25" s="44" t="s">
+      <c r="J25" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="K25" s="36"/>
-      <c r="L25" s="39" t="s">
+      <c r="K25" s="38"/>
+      <c r="L25" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2374,15 +2508,15 @@
       <c r="E26" s="10">
         <v>23</v>
       </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="48"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="36"/>
       <c r="I26" s="10">
         <v>23</v>
       </c>
-      <c r="J26" s="44"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="39"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="51"/>
     </row>
     <row r="27" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
@@ -2392,13 +2526,13 @@
       <c r="E27" s="10">
         <v>24</v>
       </c>
-      <c r="F27" s="49" t="s">
+      <c r="F27" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="H27" s="48" t="s">
+      <c r="H27" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I27" s="10">
@@ -2407,7 +2541,7 @@
       <c r="J27" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="K27" s="45" t="s">
+      <c r="K27" s="52" t="s">
         <v>160</v>
       </c>
       <c r="L27" s="32" t="s">
@@ -2422,16 +2556,16 @@
       <c r="E28" s="10">
         <v>25</v>
       </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="48"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="36"/>
       <c r="I28" s="10">
         <v>25</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="K28" s="45"/>
+      <c r="K28" s="52"/>
       <c r="L28" s="32" t="s">
         <v>86</v>
       </c>
@@ -2444,11 +2578,11 @@
       <c r="E29" s="10">
         <v>26</v>
       </c>
-      <c r="F29" s="49" t="s">
+      <c r="F29" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="36"/>
-      <c r="H29" s="48" t="s">
+      <c r="G29" s="38"/>
+      <c r="H29" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I29" s="10">
@@ -2457,7 +2591,7 @@
       <c r="J29" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="K29" s="45"/>
+      <c r="K29" s="52"/>
       <c r="L29" s="32" t="s">
         <v>86</v>
       </c>
@@ -2470,16 +2604,16 @@
       <c r="E30" s="10">
         <v>27</v>
       </c>
-      <c r="F30" s="49"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="48"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="36"/>
       <c r="I30" s="10">
         <v>27</v>
       </c>
       <c r="J30" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="K30" s="45"/>
+      <c r="K30" s="52"/>
       <c r="L30" s="32" t="s">
         <v>86</v>
       </c>
@@ -2492,21 +2626,21 @@
       <c r="E31" s="10">
         <v>28</v>
       </c>
-      <c r="F31" s="49" t="s">
+      <c r="F31" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="G31" s="36"/>
-      <c r="H31" s="48" t="s">
+      <c r="G31" s="38"/>
+      <c r="H31" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I31" s="10">
         <v>28</v>
       </c>
-      <c r="J31" s="44" t="s">
+      <c r="J31" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="K31" s="45"/>
-      <c r="L31" s="39" t="s">
+      <c r="K31" s="52"/>
+      <c r="L31" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2518,15 +2652,15 @@
       <c r="E32" s="10">
         <v>29</v>
       </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="48"/>
+      <c r="F32" s="37"/>
+      <c r="G32" s="38"/>
+      <c r="H32" s="36"/>
       <c r="I32" s="10">
         <v>29</v>
       </c>
-      <c r="J32" s="44"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="39"/>
+      <c r="J32" s="46"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="51"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
@@ -2536,21 +2670,21 @@
       <c r="E33" s="10">
         <v>30</v>
       </c>
-      <c r="F33" s="49" t="s">
+      <c r="F33" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="G33" s="36"/>
-      <c r="H33" s="48" t="s">
+      <c r="G33" s="38"/>
+      <c r="H33" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I33" s="10">
         <v>30</v>
       </c>
-      <c r="J33" s="44" t="s">
+      <c r="J33" s="46" t="s">
         <v>105</v>
       </c>
-      <c r="K33" s="45"/>
-      <c r="L33" s="39" t="s">
+      <c r="K33" s="52"/>
+      <c r="L33" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2562,15 +2696,15 @@
       <c r="E34" s="10">
         <v>31</v>
       </c>
-      <c r="F34" s="49"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="48"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="36"/>
       <c r="I34" s="10">
         <v>31</v>
       </c>
-      <c r="J34" s="44"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="39"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="51"/>
     </row>
     <row r="35" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
@@ -2580,13 +2714,13 @@
       <c r="E35" s="10">
         <v>32</v>
       </c>
-      <c r="F35" s="49" t="s">
+      <c r="F35" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G35" s="36" t="s">
+      <c r="G35" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H35" s="48" t="s">
+      <c r="H35" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I35" s="10">
@@ -2595,7 +2729,7 @@
       <c r="J35" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="K35" s="36" t="s">
+      <c r="K35" s="38" t="s">
         <v>161</v>
       </c>
       <c r="L35" s="32" t="s">
@@ -2610,16 +2744,16 @@
       <c r="E36" s="10">
         <v>33</v>
       </c>
-      <c r="F36" s="49"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="48"/>
+      <c r="F36" s="37"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="36"/>
       <c r="I36" s="10">
         <v>33</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="K36" s="36"/>
+      <c r="K36" s="38"/>
       <c r="L36" s="32" t="s">
         <v>86</v>
       </c>
@@ -2628,11 +2762,11 @@
       <c r="E37" s="10">
         <v>34</v>
       </c>
-      <c r="F37" s="49" t="s">
+      <c r="F37" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G37" s="36"/>
-      <c r="H37" s="48" t="s">
+      <c r="G37" s="38"/>
+      <c r="H37" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I37" s="10">
@@ -2641,7 +2775,7 @@
       <c r="J37" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="K37" s="36"/>
+      <c r="K37" s="38"/>
       <c r="L37" s="32" t="s">
         <v>86</v>
       </c>
@@ -2650,16 +2784,16 @@
       <c r="E38" s="10">
         <v>35</v>
       </c>
-      <c r="F38" s="49"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="48"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="36"/>
       <c r="I38" s="10">
         <v>35</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="K38" s="36"/>
+      <c r="K38" s="38"/>
       <c r="L38" s="32" t="s">
         <v>86</v>
       </c>
@@ -2668,21 +2802,21 @@
       <c r="E39" s="10">
         <v>36</v>
       </c>
-      <c r="F39" s="49" t="s">
+      <c r="F39" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="G39" s="36"/>
-      <c r="H39" s="48" t="s">
+      <c r="G39" s="38"/>
+      <c r="H39" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I39" s="10">
         <v>36</v>
       </c>
-      <c r="J39" s="44" t="s">
+      <c r="J39" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="K39" s="36"/>
-      <c r="L39" s="39" t="s">
+      <c r="K39" s="38"/>
+      <c r="L39" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2690,35 +2824,35 @@
       <c r="E40" s="10">
         <v>37</v>
       </c>
-      <c r="F40" s="49"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="48"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="36"/>
       <c r="I40" s="10">
         <v>37</v>
       </c>
-      <c r="J40" s="44"/>
-      <c r="K40" s="36"/>
-      <c r="L40" s="39"/>
+      <c r="J40" s="46"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="51"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E41" s="10">
         <v>38</v>
       </c>
-      <c r="F41" s="49" t="s">
+      <c r="F41" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="G41" s="36"/>
-      <c r="H41" s="48" t="s">
+      <c r="G41" s="38"/>
+      <c r="H41" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I41" s="10">
         <v>38</v>
       </c>
-      <c r="J41" s="44" t="s">
+      <c r="J41" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="K41" s="36"/>
-      <c r="L41" s="39" t="s">
+      <c r="K41" s="38"/>
+      <c r="L41" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2726,27 +2860,27 @@
       <c r="E42" s="10">
         <v>39</v>
       </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="48"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="36"/>
       <c r="I42" s="10">
         <v>39</v>
       </c>
-      <c r="J42" s="44"/>
-      <c r="K42" s="36"/>
-      <c r="L42" s="39"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="51"/>
     </row>
     <row r="43" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
       <c r="E43" s="10">
         <v>40</v>
       </c>
-      <c r="F43" s="49" t="s">
+      <c r="F43" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="G43" s="36" t="s">
+      <c r="G43" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I43" s="10">
@@ -2766,19 +2900,19 @@
       <c r="E44" s="10">
         <v>41</v>
       </c>
-      <c r="F44" s="49"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="48"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="36"/>
       <c r="I44" s="10">
         <v>41</v>
       </c>
-      <c r="J44" s="41" t="s">
+      <c r="J44" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="K44" s="40" t="s">
+      <c r="K44" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="L44" s="39" t="s">
+      <c r="L44" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2786,37 +2920,37 @@
       <c r="E45" s="10">
         <v>42</v>
       </c>
-      <c r="F45" s="49" t="s">
+      <c r="F45" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="G45" s="36" t="s">
+      <c r="G45" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="H45" s="48" t="s">
+      <c r="H45" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I45" s="10">
         <v>42</v>
       </c>
-      <c r="J45" s="42"/>
-      <c r="K45" s="40"/>
-      <c r="L45" s="39"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="50"/>
+      <c r="L45" s="51"/>
     </row>
     <row r="46" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E46" s="10">
         <v>43</v>
       </c>
-      <c r="F46" s="49"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="48"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="38"/>
+      <c r="H46" s="36"/>
       <c r="I46" s="10">
         <v>43</v>
       </c>
-      <c r="J46" s="41" t="s">
+      <c r="J46" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="K46" s="40"/>
-      <c r="L46" s="39" t="s">
+      <c r="K46" s="50"/>
+      <c r="L46" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2824,37 +2958,37 @@
       <c r="E47" s="10">
         <v>44</v>
       </c>
-      <c r="F47" s="49" t="s">
+      <c r="F47" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="G47" s="36" t="s">
+      <c r="G47" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="H47" s="48" t="s">
+      <c r="H47" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I47" s="10">
         <v>44</v>
       </c>
-      <c r="J47" s="42"/>
-      <c r="K47" s="40"/>
-      <c r="L47" s="39"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="50"/>
+      <c r="L47" s="51"/>
     </row>
     <row r="48" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E48" s="10">
         <v>45</v>
       </c>
-      <c r="F48" s="49"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="48"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="36"/>
       <c r="I48" s="10">
         <v>45</v>
       </c>
-      <c r="J48" s="41" t="s">
+      <c r="J48" s="53" t="s">
         <v>136</v>
       </c>
-      <c r="K48" s="40"/>
-      <c r="L48" s="39" t="s">
+      <c r="K48" s="50"/>
+      <c r="L48" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2862,39 +2996,39 @@
       <c r="E49" s="10">
         <v>46</v>
       </c>
-      <c r="F49" s="49" t="s">
+      <c r="F49" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="G49" s="36" t="s">
+      <c r="G49" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="H49" s="48" t="s">
+      <c r="H49" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I49" s="10">
         <v>46</v>
       </c>
-      <c r="J49" s="42"/>
-      <c r="K49" s="40"/>
-      <c r="L49" s="39"/>
+      <c r="J49" s="54"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="51"/>
     </row>
     <row r="50" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E50" s="10">
         <v>47</v>
       </c>
-      <c r="F50" s="49"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="48"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="36"/>
       <c r="I50" s="10">
         <v>47</v>
       </c>
-      <c r="J50" s="41" t="s">
+      <c r="J50" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="K50" s="43" t="s">
+      <c r="K50" s="55" t="s">
         <v>116</v>
       </c>
-      <c r="L50" s="39" t="s">
+      <c r="L50" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2902,79 +3036,79 @@
       <c r="E51" s="10">
         <v>48</v>
       </c>
-      <c r="F51" s="49" t="s">
+      <c r="F51" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G51" s="36" t="s">
+      <c r="G51" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="H51" s="48" t="s">
+      <c r="H51" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I51" s="10">
         <v>48</v>
       </c>
-      <c r="J51" s="42"/>
-      <c r="K51" s="43"/>
-      <c r="L51" s="39"/>
+      <c r="J51" s="54"/>
+      <c r="K51" s="55"/>
+      <c r="L51" s="51"/>
     </row>
     <row r="52" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E52" s="10">
         <v>49</v>
       </c>
-      <c r="F52" s="49"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="48"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="36"/>
       <c r="I52" s="10">
         <v>49</v>
       </c>
-      <c r="J52" s="41" t="s">
+      <c r="J52" s="53" t="s">
         <v>137</v>
       </c>
-      <c r="K52" s="40" t="s">
+      <c r="K52" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="L52" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="N52" s="37"/>
+      <c r="L52" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="N52" s="56"/>
     </row>
     <row r="53" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E53" s="10">
         <v>50</v>
       </c>
-      <c r="F53" s="49" t="s">
+      <c r="F53" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="G53" s="36" t="s">
+      <c r="G53" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="H53" s="48" t="s">
+      <c r="H53" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I53" s="10">
         <v>50</v>
       </c>
-      <c r="J53" s="42"/>
-      <c r="K53" s="40"/>
-      <c r="L53" s="39"/>
-      <c r="N53" s="38"/>
+      <c r="J53" s="54"/>
+      <c r="K53" s="50"/>
+      <c r="L53" s="51"/>
+      <c r="N53" s="57"/>
     </row>
     <row r="54" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E54" s="10">
         <v>51</v>
       </c>
-      <c r="F54" s="49"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="48"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="36"/>
       <c r="I54" s="10">
         <v>51</v>
       </c>
-      <c r="J54" s="41" t="s">
+      <c r="J54" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="K54" s="40"/>
-      <c r="L54" s="39" t="s">
+      <c r="K54" s="50"/>
+      <c r="L54" s="51" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2994,9 +3128,9 @@
       <c r="I55" s="10">
         <v>52</v>
       </c>
-      <c r="J55" s="42"/>
-      <c r="K55" s="40"/>
-      <c r="L55" s="39"/>
+      <c r="J55" s="54"/>
+      <c r="K55" s="50"/>
+      <c r="L55" s="51"/>
     </row>
     <row r="56" spans="5:15" ht="40.5" x14ac:dyDescent="0.3">
       <c r="E56" s="10">
@@ -3014,11 +3148,11 @@
       <c r="I56" s="10">
         <v>53</v>
       </c>
-      <c r="J56" s="41" t="s">
+      <c r="J56" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="K56" s="40"/>
-      <c r="L56" s="39" t="s">
+      <c r="K56" s="50"/>
+      <c r="L56" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N56" s="1"/>
@@ -3028,21 +3162,21 @@
       <c r="E57" s="10">
         <v>54</v>
       </c>
-      <c r="F57" s="49" t="s">
+      <c r="F57" s="37" t="s">
         <v>148</v>
       </c>
-      <c r="G57" s="36" t="s">
+      <c r="G57" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="H57" s="48" t="s">
+      <c r="H57" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I57" s="10">
         <v>54</v>
       </c>
-      <c r="J57" s="42"/>
-      <c r="K57" s="40"/>
-      <c r="L57" s="39"/>
+      <c r="J57" s="54"/>
+      <c r="K57" s="50"/>
+      <c r="L57" s="51"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
     </row>
@@ -3050,19 +3184,19 @@
       <c r="E58" s="10">
         <v>55</v>
       </c>
-      <c r="F58" s="49"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="48"/>
+      <c r="F58" s="37"/>
+      <c r="G58" s="38"/>
+      <c r="H58" s="36"/>
       <c r="I58" s="10">
         <v>55</v>
       </c>
-      <c r="J58" s="41" t="s">
+      <c r="J58" s="53" t="s">
         <v>118</v>
       </c>
-      <c r="K58" s="40" t="s">
+      <c r="K58" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="L58" s="39" t="s">
+      <c r="L58" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N58" s="1"/>
@@ -3072,21 +3206,21 @@
       <c r="E59" s="10">
         <v>56</v>
       </c>
-      <c r="F59" s="49" t="s">
+      <c r="F59" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="G59" s="36" t="s">
+      <c r="G59" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="H59" s="48" t="s">
+      <c r="H59" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I59" s="10">
         <v>56</v>
       </c>
-      <c r="J59" s="42"/>
-      <c r="K59" s="40"/>
-      <c r="L59" s="39"/>
+      <c r="J59" s="54"/>
+      <c r="K59" s="50"/>
+      <c r="L59" s="51"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
     </row>
@@ -3094,19 +3228,19 @@
       <c r="E60" s="10">
         <v>57</v>
       </c>
-      <c r="F60" s="49"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="48"/>
+      <c r="F60" s="37"/>
+      <c r="G60" s="38"/>
+      <c r="H60" s="36"/>
       <c r="I60" s="10">
         <v>57</v>
       </c>
-      <c r="J60" s="41" t="s">
+      <c r="J60" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="K60" s="40" t="s">
+      <c r="K60" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="L60" s="39" t="s">
+      <c r="L60" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N60" s="1"/>
@@ -3116,21 +3250,21 @@
       <c r="E61" s="10">
         <v>58</v>
       </c>
-      <c r="F61" s="49" t="s">
+      <c r="F61" s="37" t="s">
         <v>150</v>
       </c>
-      <c r="G61" s="36" t="s">
+      <c r="G61" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="H61" s="48" t="s">
+      <c r="H61" s="36" t="s">
         <v>83</v>
       </c>
       <c r="I61" s="10">
         <v>58</v>
       </c>
-      <c r="J61" s="42"/>
-      <c r="K61" s="40"/>
-      <c r="L61" s="39"/>
+      <c r="J61" s="54"/>
+      <c r="K61" s="50"/>
+      <c r="L61" s="51"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
     </row>
@@ -3138,19 +3272,19 @@
       <c r="E62" s="10">
         <v>59</v>
       </c>
-      <c r="F62" s="49"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="48"/>
+      <c r="F62" s="37"/>
+      <c r="G62" s="38"/>
+      <c r="H62" s="36"/>
       <c r="I62" s="10">
         <v>59</v>
       </c>
-      <c r="J62" s="41" t="s">
+      <c r="J62" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="K62" s="40" t="s">
+      <c r="K62" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="L62" s="39" t="s">
+      <c r="L62" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N62" s="1"/>
@@ -3172,26 +3306,26 @@
       <c r="I63" s="10">
         <v>60</v>
       </c>
-      <c r="J63" s="42"/>
-      <c r="K63" s="40"/>
-      <c r="L63" s="39"/>
+      <c r="J63" s="54"/>
+      <c r="K63" s="50"/>
+      <c r="L63" s="51"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
     </row>
     <row r="64" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E64" s="6"/>
       <c r="F64" s="2"/>
-      <c r="H64" s="46"/>
+      <c r="H64" s="49"/>
       <c r="I64" s="10">
         <v>61</v>
       </c>
-      <c r="J64" s="41" t="s">
+      <c r="J64" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="K64" s="40" t="s">
+      <c r="K64" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="L64" s="39" t="s">
+      <c r="L64" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N64" s="1"/>
@@ -3200,13 +3334,13 @@
     <row r="65" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E65" s="6"/>
       <c r="F65" s="2"/>
-      <c r="H65" s="46"/>
+      <c r="H65" s="49"/>
       <c r="I65" s="10">
         <v>62</v>
       </c>
-      <c r="J65" s="42"/>
-      <c r="K65" s="40"/>
-      <c r="L65" s="39"/>
+      <c r="J65" s="54"/>
+      <c r="K65" s="50"/>
+      <c r="L65" s="51"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
     </row>
@@ -3216,13 +3350,13 @@
       <c r="I66" s="10">
         <v>63</v>
       </c>
-      <c r="J66" s="41" t="s">
+      <c r="J66" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="K66" s="40" t="s">
+      <c r="K66" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="L66" s="39" t="s">
+      <c r="L66" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N66" s="1"/>
@@ -3233,9 +3367,9 @@
       <c r="I67" s="10">
         <v>64</v>
       </c>
-      <c r="J67" s="42"/>
-      <c r="K67" s="40"/>
-      <c r="L67" s="39"/>
+      <c r="J67" s="54"/>
+      <c r="K67" s="50"/>
+      <c r="L67" s="51"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
     </row>
@@ -3244,13 +3378,13 @@
       <c r="I68" s="10">
         <v>65</v>
       </c>
-      <c r="J68" s="41" t="s">
+      <c r="J68" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="K68" s="40" t="s">
+      <c r="K68" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="L68" s="39" t="s">
+      <c r="L68" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N68" s="1"/>
@@ -3261,9 +3395,9 @@
       <c r="I69" s="10">
         <v>66</v>
       </c>
-      <c r="J69" s="42"/>
-      <c r="K69" s="40"/>
-      <c r="L69" s="39"/>
+      <c r="J69" s="54"/>
+      <c r="K69" s="50"/>
+      <c r="L69" s="51"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
     </row>
@@ -3272,13 +3406,13 @@
       <c r="I70" s="10">
         <v>67</v>
       </c>
-      <c r="J70" s="41" t="s">
+      <c r="J70" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="K70" s="36" t="s">
+      <c r="K70" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="L70" s="39" t="s">
+      <c r="L70" s="51" t="s">
         <v>83</v>
       </c>
       <c r="N70" s="1"/>
@@ -3289,9 +3423,9 @@
       <c r="I71" s="10">
         <v>68</v>
       </c>
-      <c r="J71" s="42"/>
-      <c r="K71" s="40"/>
-      <c r="L71" s="39"/>
+      <c r="J71" s="54"/>
+      <c r="K71" s="50"/>
+      <c r="L71" s="51"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
     </row>
@@ -3305,8 +3439,8 @@
       </c>
       <c r="K72" s="13"/>
       <c r="L72" s="34"/>
-      <c r="N72" s="54"/>
-      <c r="O72" s="54"/>
+      <c r="N72" s="40"/>
+      <c r="O72" s="40"/>
     </row>
     <row r="73" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F73" s="2"/>
@@ -3318,8 +3452,8 @@
       </c>
       <c r="K73" s="13"/>
       <c r="L73" s="34"/>
-      <c r="N73" s="54"/>
-      <c r="O73" s="54"/>
+      <c r="N73" s="40"/>
+      <c r="O73" s="40"/>
     </row>
     <row r="74" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F74" s="2"/>
@@ -3331,8 +3465,8 @@
       </c>
       <c r="K74" s="13"/>
       <c r="L74" s="34"/>
-      <c r="N74" s="54"/>
-      <c r="O74" s="54"/>
+      <c r="N74" s="40"/>
+      <c r="O74" s="40"/>
     </row>
     <row r="75" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F75" s="2"/>
@@ -3344,8 +3478,8 @@
       </c>
       <c r="K75" s="13"/>
       <c r="L75" s="34"/>
-      <c r="N75" s="54"/>
-      <c r="O75" s="54"/>
+      <c r="N75" s="40"/>
+      <c r="O75" s="40"/>
     </row>
     <row r="76" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F76" s="2"/>
@@ -3357,8 +3491,8 @@
       </c>
       <c r="K76" s="13"/>
       <c r="L76" s="34"/>
-      <c r="N76" s="54"/>
-      <c r="O76" s="54"/>
+      <c r="N76" s="40"/>
+      <c r="O76" s="40"/>
     </row>
     <row r="77" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F77" s="2"/>
@@ -3370,8 +3504,8 @@
       </c>
       <c r="K77" s="13"/>
       <c r="L77" s="34"/>
-      <c r="N77" s="54"/>
-      <c r="O77" s="54"/>
+      <c r="N77" s="40"/>
+      <c r="O77" s="40"/>
     </row>
     <row r="78" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F78" s="2"/>
@@ -3409,8 +3543,8 @@
       </c>
       <c r="K80" s="13"/>
       <c r="L80" s="34"/>
-      <c r="N80" s="54"/>
-      <c r="O80" s="53"/>
+      <c r="N80" s="40"/>
+      <c r="O80" s="39"/>
     </row>
     <row r="81" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F81" s="2"/>
@@ -3422,8 +3556,8 @@
       </c>
       <c r="K81" s="13"/>
       <c r="L81" s="34"/>
-      <c r="N81" s="54"/>
-      <c r="O81" s="53"/>
+      <c r="N81" s="40"/>
+      <c r="O81" s="39"/>
     </row>
     <row r="82" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F82" s="2"/>
@@ -3435,8 +3569,8 @@
       </c>
       <c r="K82" s="13"/>
       <c r="L82" s="34"/>
-      <c r="N82" s="54"/>
-      <c r="O82" s="53"/>
+      <c r="N82" s="40"/>
+      <c r="O82" s="39"/>
     </row>
     <row r="83" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I83" s="10">
@@ -3451,8 +3585,8 @@
       <c r="L83" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="N83" s="54"/>
-      <c r="O83" s="53"/>
+      <c r="N83" s="40"/>
+      <c r="O83" s="39"/>
     </row>
     <row r="84" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I84" s="10">
@@ -3467,8 +3601,8 @@
       <c r="L84" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="N84" s="54"/>
-      <c r="O84" s="54"/>
+      <c r="N84" s="40"/>
+      <c r="O84" s="40"/>
     </row>
     <row r="85" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I85" s="10">
@@ -3483,8 +3617,8 @@
       <c r="L85" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="N85" s="54"/>
-      <c r="O85" s="54"/>
+      <c r="N85" s="40"/>
+      <c r="O85" s="40"/>
     </row>
     <row r="86" spans="6:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I86" s="10">
@@ -3493,14 +3627,14 @@
       <c r="J86" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K86" s="36" t="s">
+      <c r="K86" s="38" t="s">
         <v>127</v>
       </c>
       <c r="L86" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="N86" s="54"/>
-      <c r="O86" s="56"/>
+      <c r="N86" s="40"/>
+      <c r="O86" s="41"/>
     </row>
     <row r="87" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I87" s="10">
@@ -3509,12 +3643,12 @@
       <c r="J87" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K87" s="36"/>
+      <c r="K87" s="38"/>
       <c r="L87" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="N87" s="54"/>
-      <c r="O87" s="56"/>
+      <c r="N87" s="40"/>
+      <c r="O87" s="41"/>
     </row>
     <row r="88" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I88" s="10">
@@ -3523,12 +3657,12 @@
       <c r="J88" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K88" s="36"/>
+      <c r="K88" s="38"/>
       <c r="L88" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="N88" s="54"/>
-      <c r="O88" s="54"/>
+      <c r="N88" s="40"/>
+      <c r="O88" s="40"/>
     </row>
     <row r="89" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I89" s="10">
@@ -3537,12 +3671,12 @@
       <c r="J89" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K89" s="36"/>
+      <c r="K89" s="38"/>
       <c r="L89" s="34" t="s">
         <v>84</v>
       </c>
-      <c r="N89" s="54"/>
-      <c r="O89" s="54"/>
+      <c r="N89" s="40"/>
+      <c r="O89" s="40"/>
     </row>
     <row r="90" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I90" s="10">
@@ -3551,7 +3685,7 @@
       <c r="J90" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K90" s="36"/>
+      <c r="K90" s="38"/>
       <c r="L90" s="34" t="s">
         <v>84</v>
       </c>
@@ -3565,7 +3699,7 @@
       <c r="J91" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K91" s="36"/>
+      <c r="K91" s="38"/>
       <c r="L91" s="34" t="s">
         <v>84</v>
       </c>
@@ -3579,7 +3713,7 @@
       <c r="J92" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K92" s="36"/>
+      <c r="K92" s="38"/>
       <c r="L92" s="34" t="s">
         <v>84</v>
       </c>
@@ -3593,7 +3727,7 @@
       <c r="J93" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K93" s="36"/>
+      <c r="K93" s="38"/>
       <c r="L93" s="34" t="s">
         <v>84</v>
       </c>
@@ -3607,7 +3741,7 @@
       <c r="J94" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K94" s="36"/>
+      <c r="K94" s="38"/>
       <c r="L94" s="34" t="s">
         <v>84</v>
       </c>
@@ -3621,7 +3755,7 @@
       <c r="J95" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="K95" s="36"/>
+      <c r="K95" s="38"/>
       <c r="L95" s="34" t="s">
         <v>84</v>
       </c>
@@ -3748,37 +3882,37 @@
       <c r="I115" s="6"/>
     </row>
     <row r="135" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O135" s="53"/>
+      <c r="O135" s="39"/>
     </row>
     <row r="136" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O136" s="53"/>
+      <c r="O136" s="39"/>
     </row>
     <row r="137" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O137" s="53"/>
+      <c r="O137" s="39"/>
     </row>
     <row r="138" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O138" s="53"/>
+      <c r="O138" s="39"/>
     </row>
     <row r="139" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O139" s="53"/>
+      <c r="O139" s="39"/>
     </row>
     <row r="140" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O140" s="53"/>
+      <c r="O140" s="39"/>
     </row>
     <row r="141" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O141" s="53"/>
+      <c r="O141" s="39"/>
     </row>
     <row r="142" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O142" s="53"/>
+      <c r="O142" s="39"/>
     </row>
     <row r="143" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O143" s="53"/>
+      <c r="O143" s="39"/>
     </row>
     <row r="144" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O144" s="53"/>
+      <c r="O144" s="39"/>
     </row>
     <row r="145" spans="14:15" x14ac:dyDescent="0.3">
-      <c r="O145" s="53"/>
+      <c r="O145" s="39"/>
     </row>
     <row r="151" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N151" s="2"/>
@@ -3786,100 +3920,44 @@
     </row>
   </sheetData>
   <mergeCells count="162">
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="O135:O145"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="N72:N73"/>
-    <mergeCell ref="N74:N75"/>
-    <mergeCell ref="N76:N77"/>
-    <mergeCell ref="O72:O73"/>
-    <mergeCell ref="O74:O75"/>
-    <mergeCell ref="O76:O77"/>
-    <mergeCell ref="N80:N81"/>
-    <mergeCell ref="N82:N83"/>
-    <mergeCell ref="N84:N85"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="O80:O83"/>
-    <mergeCell ref="G35:G42"/>
-    <mergeCell ref="N86:N87"/>
-    <mergeCell ref="O86:O87"/>
-    <mergeCell ref="N88:N89"/>
-    <mergeCell ref="O88:O89"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="G11:G18"/>
-    <mergeCell ref="G19:G26"/>
-    <mergeCell ref="G27:G34"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="K86:K95"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="L62:L63"/>
+    <mergeCell ref="L64:L65"/>
+    <mergeCell ref="L66:L67"/>
+    <mergeCell ref="L68:L69"/>
+    <mergeCell ref="L70:L71"/>
+    <mergeCell ref="L52:L53"/>
+    <mergeCell ref="L54:L55"/>
+    <mergeCell ref="L56:L57"/>
+    <mergeCell ref="L58:L59"/>
+    <mergeCell ref="L60:L61"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="K52:K57"/>
+    <mergeCell ref="K58:K59"/>
+    <mergeCell ref="K60:K61"/>
+    <mergeCell ref="K62:K63"/>
+    <mergeCell ref="K64:K65"/>
+    <mergeCell ref="K66:K67"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="K35:K42"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="K44:K49"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="L46:L47"/>
+    <mergeCell ref="L48:L49"/>
+    <mergeCell ref="J44:J45"/>
     <mergeCell ref="J17:J18"/>
     <mergeCell ref="L17:L18"/>
     <mergeCell ref="K11:K18"/>
@@ -3904,50 +3982,106 @@
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="L33:L34"/>
     <mergeCell ref="J46:J47"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="G11:G18"/>
+    <mergeCell ref="G19:G26"/>
+    <mergeCell ref="G27:G34"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="O135:O145"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="N72:N73"/>
+    <mergeCell ref="N74:N75"/>
+    <mergeCell ref="N76:N77"/>
+    <mergeCell ref="O72:O73"/>
+    <mergeCell ref="O74:O75"/>
+    <mergeCell ref="O76:O77"/>
+    <mergeCell ref="N80:N81"/>
+    <mergeCell ref="N82:N83"/>
+    <mergeCell ref="N84:N85"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="O80:O83"/>
+    <mergeCell ref="N86:N87"/>
+    <mergeCell ref="O86:O87"/>
+    <mergeCell ref="N88:N89"/>
+    <mergeCell ref="O88:O89"/>
+    <mergeCell ref="H64:H65"/>
     <mergeCell ref="J48:J49"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="J52:J53"/>
-    <mergeCell ref="K35:K42"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="K44:K49"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="L46:L47"/>
-    <mergeCell ref="L48:L49"/>
     <mergeCell ref="L50:L51"/>
     <mergeCell ref="J64:J65"/>
     <mergeCell ref="J66:J67"/>
-    <mergeCell ref="J68:J69"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="K50:K51"/>
-    <mergeCell ref="K52:K57"/>
-    <mergeCell ref="K58:K59"/>
-    <mergeCell ref="K60:K61"/>
-    <mergeCell ref="K62:K63"/>
-    <mergeCell ref="K64:K65"/>
-    <mergeCell ref="K66:K67"/>
-    <mergeCell ref="K68:K69"/>
-    <mergeCell ref="K70:K71"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="J56:J57"/>
-    <mergeCell ref="J58:J59"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="J44:J45"/>
-    <mergeCell ref="K86:K95"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="L62:L63"/>
-    <mergeCell ref="L64:L65"/>
-    <mergeCell ref="L66:L67"/>
-    <mergeCell ref="L68:L69"/>
-    <mergeCell ref="L70:L71"/>
-    <mergeCell ref="L52:L53"/>
-    <mergeCell ref="L54:L55"/>
-    <mergeCell ref="L56:L57"/>
-    <mergeCell ref="L58:L59"/>
-    <mergeCell ref="L60:L61"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="G35:G42"/>
+    <mergeCell ref="H21:H22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4060,4 +4194,486 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A024F30-D2E7-4B26-8224-6638297F660F}">
+  <dimension ref="A1:B66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>178</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>184</v>
+      </c>
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>185</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>186</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>187</v>
+      </c>
+      <c r="B31">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>189</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>190</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>191</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>192</v>
+      </c>
+      <c r="B39">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>195</v>
+      </c>
+      <c r="B44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>196</v>
+      </c>
+      <c r="B46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>197</v>
+      </c>
+      <c r="B48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>198</v>
+      </c>
+      <c r="B50">
+        <v>1.12516E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>199</v>
+      </c>
+      <c r="B52">
+        <v>2.3472099999999999E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>200</v>
+      </c>
+      <c r="B54" s="58">
+        <v>8.5876999999999995E-8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>201</v>
+      </c>
+      <c r="B56">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>202</v>
+      </c>
+      <c r="B58">
+        <v>2530</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B60">
+        <v>3335</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>204</v>
+      </c>
+      <c r="B62">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>205</v>
+      </c>
+      <c r="B64">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix the uart1 halt  issue. Slow down the system led flashing speed. Update to v1.0.2
</commit_message>
<xml_diff>
--- a/通讯协议.xlsx
+++ b/通讯协议.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\Irixi\006 4x25G DML TOSA\Power Supply Board\Firmware\4x25G_DML_TOSA_PowerSupply\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Projects\Irixi\006 4x25G DML TOSA\Power Supply Board\Firmware\4x25G_DML_TOSA_PowerSupply\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1AEE69-07CF-44E5-A985-EB8388239B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968F2C0B-9367-4288-A603-0D3DD6E3E244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="214">
   <si>
     <t>Colis</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -235,12 +235,6 @@
   </si>
   <si>
     <t>TOSA I2C Address</t>
-  </si>
-  <si>
-    <t>TOSA I2C Reg</t>
-  </si>
-  <si>
-    <t>TOSA I2C Length</t>
   </si>
   <si>
     <t>TOSA I2C Data Byte</t>
@@ -891,6 +885,42 @@
   </si>
   <si>
     <t>Target Temp (C)</t>
+  </si>
+  <si>
+    <t>I2C Comm Cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I2C 通讯次数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version Major</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version Minor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version Rev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>固件版本号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOSA I2C Reg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOSA I2C Length</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOSA I2C Data Byte</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1041,7 +1071,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1129,12 +1159,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1233,14 +1274,63 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1251,55 +1341,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1806,8 +1853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O151"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J8"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1829,61 +1876,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42" t="s">
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42" t="s">
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
     </row>
     <row r="2" spans="1:12" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G2" s="21" t="s">
         <v>23</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I2" s="20" t="s">
         <v>1</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>23</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="27" x14ac:dyDescent="0.3">
@@ -1891,25 +1938,25 @@
         <v>0</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>131</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E3" s="18">
         <v>0</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>83</v>
+      <c r="G3" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>81</v>
       </c>
       <c r="I3" s="18">
         <v>0</v>
@@ -1921,7 +1968,7 @@
         <v>28</v>
       </c>
       <c r="L3" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="27" x14ac:dyDescent="0.3">
@@ -1929,18 +1976,18 @@
         <v>1</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="C4" s="48"/>
+        <v>129</v>
+      </c>
+      <c r="C4" s="52"/>
       <c r="D4" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E4" s="10">
         <v>1</v>
       </c>
       <c r="F4" s="46"/>
       <c r="G4" s="38"/>
-      <c r="H4" s="36"/>
+      <c r="H4" s="47"/>
       <c r="I4" s="10">
         <v>1</v>
       </c>
@@ -1951,7 +1998,7 @@
         <v>25</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="27" x14ac:dyDescent="0.3">
@@ -1959,23 +2006,23 @@
         <v>2</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="48"/>
+        <v>128</v>
+      </c>
+      <c r="C5" s="52"/>
       <c r="D5" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="10">
         <v>2</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="50" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="36" t="s">
-        <v>83</v>
+        <v>54</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I5" s="10">
         <v>2</v>
@@ -1987,7 +2034,7 @@
         <v>26</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -1995,20 +2042,20 @@
         <v>3</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" s="10">
         <v>3</v>
       </c>
-      <c r="F6" s="37"/>
+      <c r="F6" s="50"/>
       <c r="G6" s="38"/>
-      <c r="H6" s="36"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="10">
         <v>3</v>
       </c>
@@ -2019,7 +2066,7 @@
         <v>27</v>
       </c>
       <c r="L6" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -2027,37 +2074,37 @@
         <v>4</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E7" s="10">
         <v>4</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="50" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>83</v>
+        <v>55</v>
+      </c>
+      <c r="H7" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I7" s="10">
         <v>4</v>
       </c>
       <c r="J7" s="46" t="s">
-        <v>91</v>
-      </c>
-      <c r="K7" s="50" t="s">
-        <v>88</v>
-      </c>
-      <c r="L7" s="51" t="s">
-        <v>83</v>
+        <v>89</v>
+      </c>
+      <c r="K7" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="L7" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
@@ -2068,60 +2115,60 @@
         <v>39</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" s="10">
         <v>5</v>
       </c>
-      <c r="F8" s="37"/>
+      <c r="F8" s="50"/>
       <c r="G8" s="38"/>
-      <c r="H8" s="36"/>
+      <c r="H8" s="47"/>
       <c r="I8" s="10">
         <v>5</v>
       </c>
       <c r="J8" s="46"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="51"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="41"/>
     </row>
     <row r="9" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>6</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E9" s="10">
         <v>6</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="50" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="36" t="s">
-        <v>83</v>
+        <v>56</v>
+      </c>
+      <c r="H9" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I9" s="10">
         <v>6</v>
       </c>
       <c r="J9" s="46" t="s">
-        <v>89</v>
-      </c>
-      <c r="K9" s="50" t="s">
-        <v>90</v>
-      </c>
-      <c r="L9" s="51" t="s">
-        <v>83</v>
+        <v>87</v>
+      </c>
+      <c r="K9" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="L9" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -2132,15 +2179,15 @@
       <c r="E10" s="10">
         <v>7</v>
       </c>
-      <c r="F10" s="37"/>
+      <c r="F10" s="50"/>
       <c r="G10" s="38"/>
-      <c r="H10" s="36"/>
+      <c r="H10" s="47"/>
       <c r="I10" s="10">
         <v>7</v>
       </c>
       <c r="J10" s="46"/>
-      <c r="K10" s="50"/>
-      <c r="L10" s="51"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="41"/>
     </row>
     <row r="11" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
@@ -2150,26 +2197,26 @@
       <c r="E11" s="10">
         <v>8</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="50" t="s">
         <v>9</v>
       </c>
       <c r="G11" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="H11" s="36" t="s">
-        <v>83</v>
+        <v>57</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I11" s="10">
         <v>8</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K11" s="38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="L11" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -2180,18 +2227,18 @@
       <c r="E12" s="10">
         <v>9</v>
       </c>
-      <c r="F12" s="37"/>
+      <c r="F12" s="50"/>
       <c r="G12" s="38"/>
-      <c r="H12" s="36"/>
+      <c r="H12" s="47"/>
       <c r="I12" s="10">
         <v>9</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K12" s="38"/>
       <c r="L12" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -2202,22 +2249,22 @@
       <c r="E13" s="10">
         <v>10</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="50" t="s">
         <v>10</v>
       </c>
       <c r="G13" s="38"/>
-      <c r="H13" s="36" t="s">
-        <v>83</v>
+      <c r="H13" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I13" s="10">
         <v>10</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K13" s="38"/>
       <c r="L13" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -2228,18 +2275,18 @@
       <c r="E14" s="10">
         <v>11</v>
       </c>
-      <c r="F14" s="37"/>
+      <c r="F14" s="50"/>
       <c r="G14" s="38"/>
-      <c r="H14" s="36"/>
+      <c r="H14" s="47"/>
       <c r="I14" s="10">
         <v>11</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K14" s="38"/>
       <c r="L14" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2250,22 +2297,22 @@
       <c r="E15" s="10">
         <v>12</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="50" t="s">
         <v>11</v>
       </c>
       <c r="G15" s="38"/>
-      <c r="H15" s="36" t="s">
-        <v>83</v>
+      <c r="H15" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I15" s="10">
         <v>12</v>
       </c>
       <c r="J15" s="46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K15" s="38"/>
-      <c r="L15" s="51" t="s">
-        <v>83</v>
+      <c r="L15" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2276,15 +2323,15 @@
       <c r="E16" s="10">
         <v>13</v>
       </c>
-      <c r="F16" s="37"/>
+      <c r="F16" s="50"/>
       <c r="G16" s="38"/>
-      <c r="H16" s="36"/>
+      <c r="H16" s="47"/>
       <c r="I16" s="10">
         <v>13</v>
       </c>
       <c r="J16" s="46"/>
       <c r="K16" s="38"/>
-      <c r="L16" s="51"/>
+      <c r="L16" s="41"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
@@ -2294,22 +2341,22 @@
       <c r="E17" s="10">
         <v>14</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="50" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="38"/>
-      <c r="H17" s="36" t="s">
-        <v>83</v>
+      <c r="H17" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I17" s="10">
         <v>14</v>
       </c>
       <c r="J17" s="46" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K17" s="38"/>
-      <c r="L17" s="51" t="s">
-        <v>83</v>
+      <c r="L17" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2320,15 +2367,15 @@
       <c r="E18" s="10">
         <v>15</v>
       </c>
-      <c r="F18" s="37"/>
+      <c r="F18" s="50"/>
       <c r="G18" s="38"/>
-      <c r="H18" s="36"/>
+      <c r="H18" s="47"/>
       <c r="I18" s="10">
         <v>15</v>
       </c>
       <c r="J18" s="46"/>
       <c r="K18" s="38"/>
-      <c r="L18" s="51"/>
+      <c r="L18" s="41"/>
     </row>
     <row r="19" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
@@ -2338,14 +2385,14 @@
       <c r="E19" s="10">
         <v>16</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F19" s="50" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="H19" s="36" t="s">
-        <v>83</v>
+        <v>58</v>
+      </c>
+      <c r="H19" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I19" s="10">
         <v>16</v>
@@ -2354,10 +2401,10 @@
         <v>33</v>
       </c>
       <c r="K19" s="38" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L19" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -2368,9 +2415,9 @@
       <c r="E20" s="10">
         <v>17</v>
       </c>
-      <c r="F20" s="37"/>
+      <c r="F20" s="50"/>
       <c r="G20" s="38"/>
-      <c r="H20" s="36"/>
+      <c r="H20" s="47"/>
       <c r="I20" s="10">
         <v>17</v>
       </c>
@@ -2379,7 +2426,7 @@
       </c>
       <c r="K20" s="38"/>
       <c r="L20" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -2390,12 +2437,12 @@
       <c r="E21" s="10">
         <v>18</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="50" t="s">
         <v>13</v>
       </c>
       <c r="G21" s="38"/>
-      <c r="H21" s="36" t="s">
-        <v>83</v>
+      <c r="H21" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I21" s="10">
         <v>18</v>
@@ -2405,7 +2452,7 @@
       </c>
       <c r="K21" s="38"/>
       <c r="L21" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -2416,9 +2463,9 @@
       <c r="E22" s="10">
         <v>19</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="38"/>
-      <c r="H22" s="36"/>
+      <c r="H22" s="47"/>
       <c r="I22" s="10">
         <v>19</v>
       </c>
@@ -2427,7 +2474,7 @@
       </c>
       <c r="K22" s="38"/>
       <c r="L22" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2438,22 +2485,22 @@
       <c r="E23" s="10">
         <v>20</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="50" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="38"/>
-      <c r="H23" s="36" t="s">
-        <v>83</v>
+      <c r="H23" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I23" s="10">
         <v>20</v>
       </c>
       <c r="J23" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K23" s="38"/>
-      <c r="L23" s="51" t="s">
-        <v>83</v>
+      <c r="L23" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -2464,15 +2511,15 @@
       <c r="E24" s="10">
         <v>21</v>
       </c>
-      <c r="F24" s="37"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="38"/>
-      <c r="H24" s="36"/>
+      <c r="H24" s="47"/>
       <c r="I24" s="10">
         <v>21</v>
       </c>
       <c r="J24" s="46"/>
       <c r="K24" s="38"/>
-      <c r="L24" s="51"/>
+      <c r="L24" s="41"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
@@ -2482,22 +2529,22 @@
       <c r="E25" s="10">
         <v>22</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="50" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="38"/>
-      <c r="H25" s="36" t="s">
-        <v>83</v>
+      <c r="H25" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I25" s="10">
         <v>22</v>
       </c>
       <c r="J25" s="46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K25" s="38"/>
-      <c r="L25" s="51" t="s">
-        <v>83</v>
+      <c r="L25" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -2508,15 +2555,15 @@
       <c r="E26" s="10">
         <v>23</v>
       </c>
-      <c r="F26" s="37"/>
+      <c r="F26" s="50"/>
       <c r="G26" s="38"/>
-      <c r="H26" s="36"/>
+      <c r="H26" s="47"/>
       <c r="I26" s="10">
         <v>23</v>
       </c>
       <c r="J26" s="46"/>
       <c r="K26" s="38"/>
-      <c r="L26" s="51"/>
+      <c r="L26" s="41"/>
     </row>
     <row r="27" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
@@ -2526,26 +2573,26 @@
       <c r="E27" s="10">
         <v>24</v>
       </c>
-      <c r="F27" s="37" t="s">
+      <c r="F27" s="50" t="s">
         <v>15</v>
       </c>
       <c r="G27" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="H27" s="36" t="s">
-        <v>83</v>
+        <v>59</v>
+      </c>
+      <c r="H27" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I27" s="10">
         <v>24</v>
       </c>
       <c r="J27" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="K27" s="52" t="s">
-        <v>160</v>
+        <v>98</v>
+      </c>
+      <c r="K27" s="48" t="s">
+        <v>158</v>
       </c>
       <c r="L27" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2556,18 +2603,18 @@
       <c r="E28" s="10">
         <v>25</v>
       </c>
-      <c r="F28" s="37"/>
+      <c r="F28" s="50"/>
       <c r="G28" s="38"/>
-      <c r="H28" s="36"/>
+      <c r="H28" s="47"/>
       <c r="I28" s="10">
         <v>25</v>
       </c>
       <c r="J28" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="K28" s="52"/>
+        <v>99</v>
+      </c>
+      <c r="K28" s="48"/>
       <c r="L28" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2578,22 +2625,22 @@
       <c r="E29" s="10">
         <v>26</v>
       </c>
-      <c r="F29" s="37" t="s">
+      <c r="F29" s="50" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="38"/>
-      <c r="H29" s="36" t="s">
-        <v>83</v>
+      <c r="H29" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I29" s="10">
         <v>26</v>
       </c>
       <c r="J29" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="K29" s="52"/>
+        <v>100</v>
+      </c>
+      <c r="K29" s="48"/>
       <c r="L29" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2604,18 +2651,18 @@
       <c r="E30" s="10">
         <v>27</v>
       </c>
-      <c r="F30" s="37"/>
+      <c r="F30" s="50"/>
       <c r="G30" s="38"/>
-      <c r="H30" s="36"/>
+      <c r="H30" s="47"/>
       <c r="I30" s="10">
         <v>27</v>
       </c>
       <c r="J30" s="25" t="s">
-        <v>103</v>
-      </c>
-      <c r="K30" s="52"/>
+        <v>101</v>
+      </c>
+      <c r="K30" s="48"/>
       <c r="L30" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -2626,22 +2673,22 @@
       <c r="E31" s="10">
         <v>28</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="50" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="38"/>
-      <c r="H31" s="36" t="s">
-        <v>83</v>
+      <c r="H31" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I31" s="10">
         <v>28</v>
       </c>
       <c r="J31" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="K31" s="52"/>
-      <c r="L31" s="51" t="s">
-        <v>83</v>
+        <v>102</v>
+      </c>
+      <c r="K31" s="48"/>
+      <c r="L31" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -2652,15 +2699,15 @@
       <c r="E32" s="10">
         <v>29</v>
       </c>
-      <c r="F32" s="37"/>
+      <c r="F32" s="50"/>
       <c r="G32" s="38"/>
-      <c r="H32" s="36"/>
+      <c r="H32" s="47"/>
       <c r="I32" s="10">
         <v>29</v>
       </c>
       <c r="J32" s="46"/>
-      <c r="K32" s="52"/>
-      <c r="L32" s="51"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="41"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="6"/>
@@ -2670,22 +2717,22 @@
       <c r="E33" s="10">
         <v>30</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F33" s="50" t="s">
         <v>18</v>
       </c>
       <c r="G33" s="38"/>
-      <c r="H33" s="36" t="s">
-        <v>83</v>
+      <c r="H33" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I33" s="10">
         <v>30</v>
       </c>
       <c r="J33" s="46" t="s">
-        <v>105</v>
-      </c>
-      <c r="K33" s="52"/>
-      <c r="L33" s="51" t="s">
-        <v>83</v>
+        <v>103</v>
+      </c>
+      <c r="K33" s="48"/>
+      <c r="L33" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -2696,15 +2743,15 @@
       <c r="E34" s="10">
         <v>31</v>
       </c>
-      <c r="F34" s="37"/>
+      <c r="F34" s="50"/>
       <c r="G34" s="38"/>
-      <c r="H34" s="36"/>
+      <c r="H34" s="47"/>
       <c r="I34" s="10">
         <v>31</v>
       </c>
       <c r="J34" s="46"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="51"/>
+      <c r="K34" s="48"/>
+      <c r="L34" s="41"/>
     </row>
     <row r="35" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
@@ -2714,26 +2761,26 @@
       <c r="E35" s="10">
         <v>32</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="F35" s="50" t="s">
         <v>19</v>
       </c>
       <c r="G35" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="H35" s="36" t="s">
-        <v>83</v>
+        <v>60</v>
+      </c>
+      <c r="H35" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I35" s="10">
         <v>32</v>
       </c>
       <c r="J35" s="25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K35" s="38" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L35" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
@@ -2744,372 +2791,372 @@
       <c r="E36" s="10">
         <v>33</v>
       </c>
-      <c r="F36" s="37"/>
+      <c r="F36" s="50"/>
       <c r="G36" s="38"/>
-      <c r="H36" s="36"/>
+      <c r="H36" s="47"/>
       <c r="I36" s="10">
         <v>33</v>
       </c>
       <c r="J36" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K36" s="38"/>
       <c r="L36" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="E37" s="10">
         <v>34</v>
       </c>
-      <c r="F37" s="37" t="s">
+      <c r="F37" s="50" t="s">
         <v>20</v>
       </c>
       <c r="G37" s="38"/>
-      <c r="H37" s="36" t="s">
-        <v>83</v>
+      <c r="H37" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I37" s="10">
         <v>34</v>
       </c>
       <c r="J37" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K37" s="38"/>
       <c r="L37" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="14.25" x14ac:dyDescent="0.3">
       <c r="E38" s="10">
         <v>35</v>
       </c>
-      <c r="F38" s="37"/>
+      <c r="F38" s="50"/>
       <c r="G38" s="38"/>
-      <c r="H38" s="36"/>
+      <c r="H38" s="47"/>
       <c r="I38" s="10">
         <v>35</v>
       </c>
       <c r="J38" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K38" s="38"/>
       <c r="L38" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E39" s="10">
         <v>36</v>
       </c>
-      <c r="F39" s="37" t="s">
+      <c r="F39" s="50" t="s">
         <v>21</v>
       </c>
       <c r="G39" s="38"/>
-      <c r="H39" s="36" t="s">
-        <v>83</v>
+      <c r="H39" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I39" s="10">
         <v>36</v>
       </c>
       <c r="J39" s="46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K39" s="38"/>
-      <c r="L39" s="51" t="s">
-        <v>83</v>
+      <c r="L39" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E40" s="10">
         <v>37</v>
       </c>
-      <c r="F40" s="37"/>
+      <c r="F40" s="50"/>
       <c r="G40" s="38"/>
-      <c r="H40" s="36"/>
+      <c r="H40" s="47"/>
       <c r="I40" s="10">
         <v>37</v>
       </c>
       <c r="J40" s="46"/>
       <c r="K40" s="38"/>
-      <c r="L40" s="51"/>
+      <c r="L40" s="41"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E41" s="10">
         <v>38</v>
       </c>
-      <c r="F41" s="37" t="s">
+      <c r="F41" s="50" t="s">
         <v>22</v>
       </c>
       <c r="G41" s="38"/>
-      <c r="H41" s="36" t="s">
-        <v>83</v>
+      <c r="H41" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I41" s="10">
         <v>38</v>
       </c>
       <c r="J41" s="46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K41" s="38"/>
-      <c r="L41" s="51" t="s">
-        <v>83</v>
+      <c r="L41" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E42" s="10">
         <v>39</v>
       </c>
-      <c r="F42" s="37"/>
+      <c r="F42" s="50"/>
       <c r="G42" s="38"/>
-      <c r="H42" s="36"/>
+      <c r="H42" s="47"/>
       <c r="I42" s="10">
         <v>39</v>
       </c>
       <c r="J42" s="46"/>
       <c r="K42" s="38"/>
-      <c r="L42" s="51"/>
+      <c r="L42" s="41"/>
     </row>
     <row r="43" spans="1:12" ht="40.5" x14ac:dyDescent="0.3">
       <c r="E43" s="10">
         <v>40</v>
       </c>
-      <c r="F43" s="37" t="s">
+      <c r="F43" s="50" t="s">
         <v>37</v>
       </c>
       <c r="G43" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="H43" s="36" t="s">
-        <v>83</v>
+        <v>61</v>
+      </c>
+      <c r="H43" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I43" s="10">
         <v>40</v>
       </c>
       <c r="J43" s="22" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="L43" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E44" s="10">
         <v>41</v>
       </c>
-      <c r="F44" s="37"/>
+      <c r="F44" s="50"/>
       <c r="G44" s="38"/>
-      <c r="H44" s="36"/>
+      <c r="H44" s="47"/>
       <c r="I44" s="10">
         <v>41</v>
       </c>
-      <c r="J44" s="53" t="s">
-        <v>134</v>
-      </c>
-      <c r="K44" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="L44" s="51" t="s">
-        <v>83</v>
+      <c r="J44" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="K44" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="L44" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E45" s="10">
         <v>42</v>
       </c>
-      <c r="F45" s="37" t="s">
+      <c r="F45" s="50" t="s">
         <v>38</v>
       </c>
       <c r="G45" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="H45" s="36" t="s">
-        <v>83</v>
+        <v>62</v>
+      </c>
+      <c r="H45" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I45" s="10">
         <v>42</v>
       </c>
-      <c r="J45" s="54"/>
-      <c r="K45" s="50"/>
-      <c r="L45" s="51"/>
+      <c r="J45" s="43"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="41"/>
     </row>
     <row r="46" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E46" s="10">
         <v>43</v>
       </c>
-      <c r="F46" s="37"/>
+      <c r="F46" s="50"/>
       <c r="G46" s="38"/>
-      <c r="H46" s="36"/>
+      <c r="H46" s="47"/>
       <c r="I46" s="10">
         <v>43</v>
       </c>
-      <c r="J46" s="53" t="s">
-        <v>135</v>
-      </c>
-      <c r="K46" s="50"/>
-      <c r="L46" s="51" t="s">
-        <v>83</v>
+      <c r="J46" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="K46" s="45"/>
+      <c r="L46" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E47" s="10">
         <v>44</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="50" t="s">
         <v>42</v>
       </c>
       <c r="G47" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="H47" s="36" t="s">
-        <v>83</v>
+        <v>63</v>
+      </c>
+      <c r="H47" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I47" s="10">
         <v>44</v>
       </c>
-      <c r="J47" s="54"/>
-      <c r="K47" s="50"/>
-      <c r="L47" s="51"/>
+      <c r="J47" s="43"/>
+      <c r="K47" s="45"/>
+      <c r="L47" s="41"/>
     </row>
     <row r="48" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E48" s="10">
         <v>45</v>
       </c>
-      <c r="F48" s="37"/>
+      <c r="F48" s="50"/>
       <c r="G48" s="38"/>
-      <c r="H48" s="36"/>
+      <c r="H48" s="47"/>
       <c r="I48" s="10">
         <v>45</v>
       </c>
-      <c r="J48" s="53" t="s">
-        <v>136</v>
-      </c>
-      <c r="K48" s="50"/>
-      <c r="L48" s="51" t="s">
-        <v>83</v>
+      <c r="J48" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="K48" s="45"/>
+      <c r="L48" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E49" s="10">
         <v>46</v>
       </c>
-      <c r="F49" s="37" t="s">
+      <c r="F49" s="50" t="s">
         <v>41</v>
       </c>
       <c r="G49" s="38" t="s">
-        <v>66</v>
-      </c>
-      <c r="H49" s="36" t="s">
-        <v>83</v>
+        <v>64</v>
+      </c>
+      <c r="H49" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I49" s="10">
         <v>46</v>
       </c>
-      <c r="J49" s="54"/>
-      <c r="K49" s="50"/>
-      <c r="L49" s="51"/>
+      <c r="J49" s="43"/>
+      <c r="K49" s="45"/>
+      <c r="L49" s="41"/>
     </row>
     <row r="50" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E50" s="10">
         <v>47</v>
       </c>
-      <c r="F50" s="37"/>
+      <c r="F50" s="50"/>
       <c r="G50" s="38"/>
-      <c r="H50" s="36"/>
+      <c r="H50" s="47"/>
       <c r="I50" s="10">
         <v>47</v>
       </c>
-      <c r="J50" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="K50" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="L50" s="51" t="s">
-        <v>83</v>
+      <c r="J50" s="42" t="s">
+        <v>144</v>
+      </c>
+      <c r="K50" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="L50" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E51" s="10">
         <v>48</v>
       </c>
-      <c r="F51" s="37" t="s">
-        <v>67</v>
+      <c r="F51" s="50" t="s">
+        <v>65</v>
       </c>
       <c r="G51" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="H51" s="36" t="s">
-        <v>83</v>
+        <v>66</v>
+      </c>
+      <c r="H51" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I51" s="10">
         <v>48</v>
       </c>
-      <c r="J51" s="54"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="51"/>
+      <c r="J51" s="43"/>
+      <c r="K51" s="44"/>
+      <c r="L51" s="41"/>
     </row>
     <row r="52" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E52" s="10">
         <v>49</v>
       </c>
-      <c r="F52" s="37"/>
+      <c r="F52" s="50"/>
       <c r="G52" s="38"/>
-      <c r="H52" s="36"/>
+      <c r="H52" s="47"/>
       <c r="I52" s="10">
         <v>49</v>
       </c>
-      <c r="J52" s="53" t="s">
-        <v>137</v>
-      </c>
-      <c r="K52" s="50" t="s">
-        <v>115</v>
-      </c>
-      <c r="L52" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="N52" s="56"/>
+      <c r="J52" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="K52" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="L52" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="N52" s="39"/>
     </row>
     <row r="53" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E53" s="10">
         <v>50</v>
       </c>
-      <c r="F53" s="37" t="s">
-        <v>69</v>
+      <c r="F53" s="50" t="s">
+        <v>67</v>
       </c>
       <c r="G53" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="H53" s="36" t="s">
-        <v>83</v>
+        <v>68</v>
+      </c>
+      <c r="H53" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I53" s="10">
         <v>50</v>
       </c>
-      <c r="J53" s="54"/>
-      <c r="K53" s="50"/>
-      <c r="L53" s="51"/>
-      <c r="N53" s="57"/>
+      <c r="J53" s="43"/>
+      <c r="K53" s="45"/>
+      <c r="L53" s="41"/>
+      <c r="N53" s="40"/>
     </row>
     <row r="54" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E54" s="10">
         <v>51</v>
       </c>
-      <c r="F54" s="37"/>
+      <c r="F54" s="50"/>
       <c r="G54" s="38"/>
-      <c r="H54" s="36"/>
+      <c r="H54" s="47"/>
       <c r="I54" s="10">
         <v>51</v>
       </c>
-      <c r="J54" s="53" t="s">
-        <v>138</v>
-      </c>
-      <c r="K54" s="50"/>
-      <c r="L54" s="51" t="s">
-        <v>83</v>
+      <c r="J54" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="K54" s="45"/>
+      <c r="L54" s="41" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="5:15" ht="40.5" x14ac:dyDescent="0.3">
@@ -3117,43 +3164,43 @@
         <v>52</v>
       </c>
       <c r="F55" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G55" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="G55" s="11" t="s">
-        <v>73</v>
-      </c>
       <c r="H55" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I55" s="10">
         <v>52</v>
       </c>
-      <c r="J55" s="54"/>
-      <c r="K55" s="50"/>
-      <c r="L55" s="51"/>
+      <c r="J55" s="43"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="41"/>
     </row>
     <row r="56" spans="5:15" ht="40.5" x14ac:dyDescent="0.3">
       <c r="E56" s="10">
         <v>53</v>
       </c>
       <c r="F56" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G56" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G56" s="11" t="s">
-        <v>74</v>
-      </c>
       <c r="H56" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I56" s="10">
         <v>53</v>
       </c>
-      <c r="J56" s="53" t="s">
-        <v>139</v>
-      </c>
-      <c r="K56" s="50"/>
-      <c r="L56" s="51" t="s">
-        <v>83</v>
+      <c r="J56" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="K56" s="45"/>
+      <c r="L56" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -3162,21 +3209,21 @@
       <c r="E57" s="10">
         <v>54</v>
       </c>
-      <c r="F57" s="37" t="s">
-        <v>148</v>
+      <c r="F57" s="50" t="s">
+        <v>146</v>
       </c>
       <c r="G57" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="H57" s="36" t="s">
-        <v>83</v>
+        <v>73</v>
+      </c>
+      <c r="H57" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I57" s="10">
         <v>54</v>
       </c>
-      <c r="J57" s="54"/>
-      <c r="K57" s="50"/>
-      <c r="L57" s="51"/>
+      <c r="J57" s="43"/>
+      <c r="K57" s="45"/>
+      <c r="L57" s="41"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
     </row>
@@ -3184,20 +3231,20 @@
       <c r="E58" s="10">
         <v>55</v>
       </c>
-      <c r="F58" s="37"/>
+      <c r="F58" s="50"/>
       <c r="G58" s="38"/>
-      <c r="H58" s="36"/>
+      <c r="H58" s="47"/>
       <c r="I58" s="10">
         <v>55</v>
       </c>
-      <c r="J58" s="53" t="s">
-        <v>118</v>
-      </c>
-      <c r="K58" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="L58" s="51" t="s">
-        <v>83</v>
+      <c r="J58" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="K58" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="L58" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="N58" s="1"/>
       <c r="O58" s="1"/>
@@ -3206,21 +3253,21 @@
       <c r="E59" s="10">
         <v>56</v>
       </c>
-      <c r="F59" s="37" t="s">
-        <v>149</v>
+      <c r="F59" s="50" t="s">
+        <v>147</v>
       </c>
       <c r="G59" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="H59" s="36" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+      <c r="H59" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I59" s="10">
         <v>56</v>
       </c>
-      <c r="J59" s="54"/>
-      <c r="K59" s="50"/>
-      <c r="L59" s="51"/>
+      <c r="J59" s="43"/>
+      <c r="K59" s="45"/>
+      <c r="L59" s="41"/>
       <c r="N59" s="1"/>
       <c r="O59" s="1"/>
     </row>
@@ -3228,20 +3275,20 @@
       <c r="E60" s="10">
         <v>57</v>
       </c>
-      <c r="F60" s="37"/>
+      <c r="F60" s="50"/>
       <c r="G60" s="38"/>
-      <c r="H60" s="36"/>
+      <c r="H60" s="47"/>
       <c r="I60" s="10">
         <v>57</v>
       </c>
-      <c r="J60" s="53" t="s">
-        <v>140</v>
-      </c>
-      <c r="K60" s="50" t="s">
-        <v>120</v>
-      </c>
-      <c r="L60" s="51" t="s">
-        <v>83</v>
+      <c r="J60" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="K60" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="L60" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="N60" s="1"/>
       <c r="O60" s="1"/>
@@ -3250,21 +3297,21 @@
       <c r="E61" s="10">
         <v>58</v>
       </c>
-      <c r="F61" s="37" t="s">
-        <v>150</v>
+      <c r="F61" s="50" t="s">
+        <v>148</v>
       </c>
       <c r="G61" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="H61" s="36" t="s">
-        <v>83</v>
+        <v>75</v>
+      </c>
+      <c r="H61" s="47" t="s">
+        <v>81</v>
       </c>
       <c r="I61" s="10">
         <v>58</v>
       </c>
-      <c r="J61" s="54"/>
-      <c r="K61" s="50"/>
-      <c r="L61" s="51"/>
+      <c r="J61" s="43"/>
+      <c r="K61" s="45"/>
+      <c r="L61" s="41"/>
       <c r="N61" s="1"/>
       <c r="O61" s="1"/>
     </row>
@@ -3272,20 +3319,20 @@
       <c r="E62" s="10">
         <v>59</v>
       </c>
-      <c r="F62" s="37"/>
+      <c r="F62" s="50"/>
       <c r="G62" s="38"/>
-      <c r="H62" s="36"/>
+      <c r="H62" s="47"/>
       <c r="I62" s="10">
         <v>59</v>
       </c>
-      <c r="J62" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="K62" s="50" t="s">
-        <v>121</v>
-      </c>
-      <c r="L62" s="51" t="s">
-        <v>83</v>
+      <c r="J62" s="42" t="s">
+        <v>139</v>
+      </c>
+      <c r="K62" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="L62" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="N62" s="1"/>
       <c r="O62" s="1"/>
@@ -3295,81 +3342,116 @@
         <v>60</v>
       </c>
       <c r="F63" s="25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G63" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H63" s="30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I63" s="10">
         <v>60</v>
       </c>
-      <c r="J63" s="54"/>
-      <c r="K63" s="50"/>
-      <c r="L63" s="51"/>
+      <c r="J63" s="43"/>
+      <c r="K63" s="45"/>
+      <c r="L63" s="41"/>
       <c r="N63" s="1"/>
       <c r="O63" s="1"/>
     </row>
-    <row r="64" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E64" s="6"/>
-      <c r="F64" s="2"/>
-      <c r="H64" s="49"/>
+    <row r="64" spans="5:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E64" s="10">
+        <v>61</v>
+      </c>
+      <c r="F64" s="36" t="s">
+        <v>205</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H64" s="30" t="s">
+        <v>82</v>
+      </c>
       <c r="I64" s="10">
         <v>61</v>
       </c>
-      <c r="J64" s="53" t="s">
-        <v>142</v>
-      </c>
-      <c r="K64" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="L64" s="51" t="s">
-        <v>83</v>
+      <c r="J64" s="42" t="s">
+        <v>140</v>
+      </c>
+      <c r="K64" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="L64" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="N64" s="1"/>
       <c r="O64" s="1"/>
     </row>
-    <row r="65" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E65" s="6"/>
-      <c r="F65" s="2"/>
-      <c r="H65" s="49"/>
+    <row r="65" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E65" s="10">
+        <v>62</v>
+      </c>
+      <c r="F65" s="36" t="s">
+        <v>207</v>
+      </c>
+      <c r="G65" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="H65" s="30" t="s">
+        <v>82</v>
+      </c>
       <c r="I65" s="10">
         <v>62</v>
       </c>
-      <c r="J65" s="54"/>
-      <c r="K65" s="50"/>
-      <c r="L65" s="51"/>
+      <c r="J65" s="43"/>
+      <c r="K65" s="45"/>
+      <c r="L65" s="41"/>
       <c r="N65" s="1"/>
       <c r="O65" s="1"/>
     </row>
-    <row r="66" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E66" s="6"/>
-      <c r="F66" s="2"/>
+    <row r="66" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E66" s="10">
+        <v>63</v>
+      </c>
+      <c r="F66" s="36" t="s">
+        <v>208</v>
+      </c>
+      <c r="G66" s="60"/>
+      <c r="H66" s="30" t="s">
+        <v>82</v>
+      </c>
       <c r="I66" s="10">
         <v>63</v>
       </c>
-      <c r="J66" s="53" t="s">
-        <v>143</v>
-      </c>
-      <c r="K66" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="L66" s="51" t="s">
-        <v>83</v>
+      <c r="J66" s="42" t="s">
+        <v>141</v>
+      </c>
+      <c r="K66" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="L66" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="N66" s="1"/>
       <c r="O66" s="1"/>
     </row>
-    <row r="67" spans="5:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F67" s="2"/>
+    <row r="67" spans="5:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E67" s="10">
+        <v>64</v>
+      </c>
+      <c r="F67" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="G67" s="54"/>
+      <c r="H67" s="30" t="s">
+        <v>82</v>
+      </c>
       <c r="I67" s="10">
         <v>64</v>
       </c>
-      <c r="J67" s="54"/>
-      <c r="K67" s="50"/>
-      <c r="L67" s="51"/>
+      <c r="J67" s="43"/>
+      <c r="K67" s="45"/>
+      <c r="L67" s="41"/>
       <c r="N67" s="1"/>
       <c r="O67" s="1"/>
     </row>
@@ -3378,14 +3460,14 @@
       <c r="I68" s="10">
         <v>65</v>
       </c>
-      <c r="J68" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="K68" s="50" t="s">
-        <v>124</v>
-      </c>
-      <c r="L68" s="51" t="s">
-        <v>83</v>
+      <c r="J68" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="K68" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="L68" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
@@ -3395,9 +3477,9 @@
       <c r="I69" s="10">
         <v>66</v>
       </c>
-      <c r="J69" s="54"/>
-      <c r="K69" s="50"/>
-      <c r="L69" s="51"/>
+      <c r="J69" s="43"/>
+      <c r="K69" s="45"/>
+      <c r="L69" s="41"/>
       <c r="N69" s="1"/>
       <c r="O69" s="1"/>
     </row>
@@ -3406,14 +3488,14 @@
       <c r="I70" s="10">
         <v>67</v>
       </c>
-      <c r="J70" s="53" t="s">
-        <v>145</v>
+      <c r="J70" s="42" t="s">
+        <v>143</v>
       </c>
       <c r="K70" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="L70" s="51" t="s">
-        <v>83</v>
+        <v>123</v>
+      </c>
+      <c r="L70" s="41" t="s">
+        <v>81</v>
       </c>
       <c r="N70" s="1"/>
       <c r="O70" s="1"/>
@@ -3423,9 +3505,9 @@
       <c r="I71" s="10">
         <v>68</v>
       </c>
-      <c r="J71" s="54"/>
-      <c r="K71" s="50"/>
-      <c r="L71" s="51"/>
+      <c r="J71" s="43"/>
+      <c r="K71" s="45"/>
+      <c r="L71" s="41"/>
       <c r="N71" s="1"/>
       <c r="O71" s="1"/>
     </row>
@@ -3435,12 +3517,12 @@
         <v>69</v>
       </c>
       <c r="J72" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K72" s="13"/>
       <c r="L72" s="34"/>
-      <c r="N72" s="40"/>
-      <c r="O72" s="40"/>
+      <c r="N72" s="57"/>
+      <c r="O72" s="57"/>
     </row>
     <row r="73" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F73" s="2"/>
@@ -3448,12 +3530,12 @@
         <v>70</v>
       </c>
       <c r="J73" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K73" s="13"/>
       <c r="L73" s="34"/>
-      <c r="N73" s="40"/>
-      <c r="O73" s="40"/>
+      <c r="N73" s="57"/>
+      <c r="O73" s="57"/>
     </row>
     <row r="74" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F74" s="2"/>
@@ -3461,12 +3543,12 @@
         <v>71</v>
       </c>
       <c r="J74" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K74" s="13"/>
       <c r="L74" s="34"/>
-      <c r="N74" s="40"/>
-      <c r="O74" s="40"/>
+      <c r="N74" s="57"/>
+      <c r="O74" s="57"/>
     </row>
     <row r="75" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F75" s="2"/>
@@ -3474,12 +3556,12 @@
         <v>72</v>
       </c>
       <c r="J75" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K75" s="13"/>
       <c r="L75" s="34"/>
-      <c r="N75" s="40"/>
-      <c r="O75" s="40"/>
+      <c r="N75" s="57"/>
+      <c r="O75" s="57"/>
     </row>
     <row r="76" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F76" s="2"/>
@@ -3487,12 +3569,12 @@
         <v>73</v>
       </c>
       <c r="J76" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K76" s="13"/>
       <c r="L76" s="34"/>
-      <c r="N76" s="40"/>
-      <c r="O76" s="40"/>
+      <c r="N76" s="57"/>
+      <c r="O76" s="57"/>
     </row>
     <row r="77" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F77" s="2"/>
@@ -3500,12 +3582,12 @@
         <v>74</v>
       </c>
       <c r="J77" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K77" s="13"/>
       <c r="L77" s="34"/>
-      <c r="N77" s="40"/>
-      <c r="O77" s="40"/>
+      <c r="N77" s="57"/>
+      <c r="O77" s="57"/>
     </row>
     <row r="78" spans="5:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F78" s="2"/>
@@ -3513,7 +3595,7 @@
         <v>75</v>
       </c>
       <c r="J78" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K78" s="13"/>
       <c r="L78" s="34"/>
@@ -3526,7 +3608,7 @@
         <v>76</v>
       </c>
       <c r="J79" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K79" s="13"/>
       <c r="L79" s="34"/>
@@ -3539,12 +3621,12 @@
         <v>77</v>
       </c>
       <c r="J80" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K80" s="13"/>
       <c r="L80" s="34"/>
-      <c r="N80" s="40"/>
-      <c r="O80" s="39"/>
+      <c r="N80" s="57"/>
+      <c r="O80" s="56"/>
     </row>
     <row r="81" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F81" s="2"/>
@@ -3552,12 +3634,12 @@
         <v>78</v>
       </c>
       <c r="J81" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K81" s="13"/>
       <c r="L81" s="34"/>
-      <c r="N81" s="40"/>
-      <c r="O81" s="39"/>
+      <c r="N81" s="57"/>
+      <c r="O81" s="56"/>
     </row>
     <row r="82" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="F82" s="2"/>
@@ -3565,12 +3647,12 @@
         <v>79</v>
       </c>
       <c r="J82" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K82" s="13"/>
       <c r="L82" s="34"/>
-      <c r="N82" s="40"/>
-      <c r="O82" s="39"/>
+      <c r="N82" s="57"/>
+      <c r="O82" s="56"/>
     </row>
     <row r="83" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I83" s="10">
@@ -3580,114 +3662,114 @@
         <v>43</v>
       </c>
       <c r="K83" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L83" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="N83" s="40"/>
-      <c r="O83" s="39"/>
+        <v>82</v>
+      </c>
+      <c r="N83" s="57"/>
+      <c r="O83" s="56"/>
     </row>
     <row r="84" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I84" s="10">
         <v>81</v>
       </c>
       <c r="J84" s="25" t="s">
-        <v>44</v>
+        <v>211</v>
       </c>
       <c r="K84" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="L84" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="N84" s="40"/>
-      <c r="O84" s="40"/>
+        <v>82</v>
+      </c>
+      <c r="N84" s="57"/>
+      <c r="O84" s="57"/>
     </row>
     <row r="85" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I85" s="10">
         <v>82</v>
       </c>
       <c r="J85" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="K85" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="K85" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="L85" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="N85" s="40"/>
-      <c r="O85" s="40"/>
+        <v>82</v>
+      </c>
+      <c r="N85" s="57"/>
+      <c r="O85" s="57"/>
     </row>
     <row r="86" spans="6:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I86" s="10">
         <v>83</v>
       </c>
       <c r="J86" s="25" t="s">
-        <v>46</v>
+        <v>213</v>
       </c>
       <c r="K86" s="38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L86" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="N86" s="40"/>
-      <c r="O86" s="41"/>
+        <v>82</v>
+      </c>
+      <c r="N86" s="57"/>
+      <c r="O86" s="58"/>
     </row>
     <row r="87" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I87" s="10">
         <v>84</v>
       </c>
       <c r="J87" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K87" s="38"/>
       <c r="L87" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="N87" s="40"/>
-      <c r="O87" s="41"/>
+        <v>82</v>
+      </c>
+      <c r="N87" s="57"/>
+      <c r="O87" s="58"/>
     </row>
     <row r="88" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I88" s="10">
         <v>85</v>
       </c>
       <c r="J88" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K88" s="38"/>
       <c r="L88" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="N88" s="40"/>
-      <c r="O88" s="40"/>
+        <v>82</v>
+      </c>
+      <c r="N88" s="57"/>
+      <c r="O88" s="57"/>
     </row>
     <row r="89" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I89" s="10">
         <v>86</v>
       </c>
       <c r="J89" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K89" s="38"/>
       <c r="L89" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="N89" s="40"/>
-      <c r="O89" s="40"/>
+        <v>82</v>
+      </c>
+      <c r="N89" s="57"/>
+      <c r="O89" s="57"/>
     </row>
     <row r="90" spans="6:15" ht="14.25" x14ac:dyDescent="0.3">
       <c r="I90" s="10">
         <v>87</v>
       </c>
       <c r="J90" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K90" s="38"/>
       <c r="L90" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N90" s="1"/>
       <c r="O90" s="2"/>
@@ -3697,11 +3779,11 @@
         <v>88</v>
       </c>
       <c r="J91" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K91" s="38"/>
       <c r="L91" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N91" s="1"/>
       <c r="O91" s="1"/>
@@ -3711,11 +3793,11 @@
         <v>89</v>
       </c>
       <c r="J92" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K92" s="38"/>
       <c r="L92" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N92" s="1"/>
       <c r="O92" s="1"/>
@@ -3725,11 +3807,11 @@
         <v>90</v>
       </c>
       <c r="J93" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K93" s="38"/>
       <c r="L93" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N93" s="1"/>
       <c r="O93" s="1"/>
@@ -3739,11 +3821,11 @@
         <v>91</v>
       </c>
       <c r="J94" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K94" s="38"/>
       <c r="L94" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N94" s="1"/>
       <c r="O94" s="1"/>
@@ -3753,11 +3835,11 @@
         <v>92</v>
       </c>
       <c r="J95" s="25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K95" s="38"/>
       <c r="L95" s="34" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="N95" s="1"/>
       <c r="O95" s="1"/>
@@ -3767,7 +3849,7 @@
         <v>93</v>
       </c>
       <c r="J96" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K96" s="11"/>
       <c r="L96" s="34"/>
@@ -3777,7 +3859,7 @@
         <v>94</v>
       </c>
       <c r="J97" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K97" s="9"/>
       <c r="L97" s="34"/>
@@ -3787,7 +3869,7 @@
         <v>95</v>
       </c>
       <c r="J98" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K98" s="9"/>
       <c r="L98" s="34"/>
@@ -3797,7 +3879,7 @@
         <v>96</v>
       </c>
       <c r="J99" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K99" s="9"/>
       <c r="L99" s="34"/>
@@ -3807,7 +3889,7 @@
         <v>97</v>
       </c>
       <c r="J100" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K100" s="9"/>
       <c r="L100" s="34"/>
@@ -3817,7 +3899,7 @@
         <v>98</v>
       </c>
       <c r="J101" s="35" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K101" s="9"/>
       <c r="L101" s="34"/>
@@ -3827,13 +3909,13 @@
         <v>99</v>
       </c>
       <c r="J102" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="K102" s="16" t="s">
         <v>40</v>
       </c>
       <c r="L102" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="103" spans="9:13" x14ac:dyDescent="0.3">
@@ -3882,37 +3964,37 @@
       <c r="I115" s="6"/>
     </row>
     <row r="135" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O135" s="39"/>
+      <c r="O135" s="56"/>
     </row>
     <row r="136" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O136" s="39"/>
+      <c r="O136" s="56"/>
     </row>
     <row r="137" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O137" s="39"/>
+      <c r="O137" s="56"/>
     </row>
     <row r="138" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O138" s="39"/>
+      <c r="O138" s="56"/>
     </row>
     <row r="139" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O139" s="39"/>
+      <c r="O139" s="56"/>
     </row>
     <row r="140" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O140" s="39"/>
+      <c r="O140" s="56"/>
     </row>
     <row r="141" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O141" s="39"/>
+      <c r="O141" s="56"/>
     </row>
     <row r="142" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O142" s="39"/>
+      <c r="O142" s="56"/>
     </row>
     <row r="143" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O143" s="39"/>
+      <c r="O143" s="56"/>
     </row>
     <row r="144" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O144" s="39"/>
+      <c r="O144" s="56"/>
     </row>
     <row r="145" spans="14:15" x14ac:dyDescent="0.3">
-      <c r="O145" s="39"/>
+      <c r="O145" s="56"/>
     </row>
     <row r="151" spans="14:15" x14ac:dyDescent="0.3">
       <c r="N151" s="2"/>
@@ -3920,44 +4002,106 @@
     </row>
   </sheetData>
   <mergeCells count="162">
-    <mergeCell ref="K86:K95"/>
-    <mergeCell ref="N52:N53"/>
-    <mergeCell ref="L62:L63"/>
-    <mergeCell ref="L64:L65"/>
-    <mergeCell ref="L66:L67"/>
-    <mergeCell ref="L68:L69"/>
-    <mergeCell ref="L70:L71"/>
-    <mergeCell ref="L52:L53"/>
-    <mergeCell ref="L54:L55"/>
-    <mergeCell ref="L56:L57"/>
-    <mergeCell ref="L58:L59"/>
-    <mergeCell ref="L60:L61"/>
-    <mergeCell ref="J68:J69"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="K50:K51"/>
-    <mergeCell ref="K52:K57"/>
-    <mergeCell ref="K58:K59"/>
-    <mergeCell ref="K60:K61"/>
-    <mergeCell ref="K62:K63"/>
-    <mergeCell ref="K64:K65"/>
-    <mergeCell ref="K66:K67"/>
-    <mergeCell ref="K68:K69"/>
-    <mergeCell ref="K70:K71"/>
-    <mergeCell ref="J54:J55"/>
-    <mergeCell ref="J56:J57"/>
-    <mergeCell ref="J58:J59"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="K35:K42"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="K44:K49"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="L46:L47"/>
-    <mergeCell ref="L48:L49"/>
-    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="G65:G67"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G47:G48"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="G35:G42"/>
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="O135:O145"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="N72:N73"/>
+    <mergeCell ref="N74:N75"/>
+    <mergeCell ref="N76:N77"/>
+    <mergeCell ref="O72:O73"/>
+    <mergeCell ref="O74:O75"/>
+    <mergeCell ref="O76:O77"/>
+    <mergeCell ref="N80:N81"/>
+    <mergeCell ref="N82:N83"/>
+    <mergeCell ref="N84:N85"/>
+    <mergeCell ref="O84:O85"/>
+    <mergeCell ref="O80:O83"/>
+    <mergeCell ref="N86:N87"/>
+    <mergeCell ref="O86:O87"/>
+    <mergeCell ref="N88:N89"/>
+    <mergeCell ref="O88:O89"/>
+    <mergeCell ref="J48:J49"/>
+    <mergeCell ref="J50:J51"/>
+    <mergeCell ref="J52:J53"/>
+    <mergeCell ref="L50:L51"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="F61:F62"/>
+    <mergeCell ref="G61:G62"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="G11:G18"/>
+    <mergeCell ref="G19:G26"/>
+    <mergeCell ref="G27:G34"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="F49:F50"/>
+    <mergeCell ref="H31:H32"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="F57:F58"/>
+    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="L9:L10"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="L15:L16"/>
     <mergeCell ref="J17:J18"/>
     <mergeCell ref="L17:L18"/>
     <mergeCell ref="K11:K18"/>
@@ -3982,106 +4126,44 @@
     <mergeCell ref="J33:J34"/>
     <mergeCell ref="L33:L34"/>
     <mergeCell ref="J46:J47"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="L9:L10"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="H31:H32"/>
-    <mergeCell ref="H33:H34"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="G11:G18"/>
-    <mergeCell ref="G19:G26"/>
-    <mergeCell ref="G27:G34"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="H25:H26"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="O135:O145"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="N72:N73"/>
-    <mergeCell ref="N74:N75"/>
-    <mergeCell ref="N76:N77"/>
-    <mergeCell ref="O72:O73"/>
-    <mergeCell ref="O74:O75"/>
-    <mergeCell ref="O76:O77"/>
-    <mergeCell ref="N80:N81"/>
-    <mergeCell ref="N82:N83"/>
-    <mergeCell ref="N84:N85"/>
-    <mergeCell ref="O84:O85"/>
-    <mergeCell ref="O80:O83"/>
-    <mergeCell ref="N86:N87"/>
-    <mergeCell ref="O86:O87"/>
-    <mergeCell ref="N88:N89"/>
-    <mergeCell ref="O88:O89"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="J48:J49"/>
-    <mergeCell ref="J50:J51"/>
-    <mergeCell ref="J52:J53"/>
-    <mergeCell ref="L50:L51"/>
-    <mergeCell ref="J64:J65"/>
-    <mergeCell ref="J66:J67"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="G35:G42"/>
-    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="K35:K42"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="K44:K49"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="L46:L47"/>
+    <mergeCell ref="L48:L49"/>
+    <mergeCell ref="J44:J45"/>
+    <mergeCell ref="J68:J69"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="K50:K51"/>
+    <mergeCell ref="K52:K57"/>
+    <mergeCell ref="K58:K59"/>
+    <mergeCell ref="K60:K61"/>
+    <mergeCell ref="K62:K63"/>
+    <mergeCell ref="K64:K65"/>
+    <mergeCell ref="K66:K67"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="J54:J55"/>
+    <mergeCell ref="J56:J57"/>
+    <mergeCell ref="J58:J59"/>
+    <mergeCell ref="J60:J61"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="K86:K95"/>
+    <mergeCell ref="N52:N53"/>
+    <mergeCell ref="L62:L63"/>
+    <mergeCell ref="L64:L65"/>
+    <mergeCell ref="L66:L67"/>
+    <mergeCell ref="L68:L69"/>
+    <mergeCell ref="L70:L71"/>
+    <mergeCell ref="L52:L53"/>
+    <mergeCell ref="L54:L55"/>
+    <mergeCell ref="L56:L57"/>
+    <mergeCell ref="L58:L59"/>
+    <mergeCell ref="L60:L61"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -4110,10 +4192,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4121,7 +4203,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4129,7 +4211,7 @@
         <v>-10</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4137,7 +4219,7 @@
         <v>-11</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4145,7 +4227,7 @@
         <v>-12</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4153,7 +4235,7 @@
         <v>-13</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4161,7 +4243,7 @@
         <v>-14</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4169,7 +4251,7 @@
         <v>-20</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -4177,7 +4259,7 @@
         <v>-21</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4200,8 +4282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A024F30-D2E7-4B26-8224-6638297F660F}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4212,7 +4294,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B1">
         <v>7</v>
@@ -4220,7 +4302,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -4228,7 +4310,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -4236,7 +4318,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -4244,7 +4326,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5">
         <v>0.5</v>
@@ -4252,12 +4334,12 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B7">
         <v>0.1</v>
@@ -4265,12 +4347,12 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -4278,7 +4360,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B10">
         <v>4</v>
@@ -4286,7 +4368,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -4294,7 +4376,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -4302,7 +4384,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B13">
         <v>0.5</v>
@@ -4310,12 +4392,12 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B15">
         <v>0.1</v>
@@ -4323,12 +4405,12 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -4336,7 +4418,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B18">
         <v>4</v>
@@ -4344,7 +4426,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B19">
         <v>4</v>
@@ -4352,7 +4434,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B20">
         <v>3</v>
@@ -4360,7 +4442,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B21">
         <v>0.5</v>
@@ -4368,12 +4450,12 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B23">
         <v>0.1</v>
@@ -4381,12 +4463,12 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B25">
         <v>7</v>
@@ -4394,7 +4476,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B26">
         <v>4</v>
@@ -4402,7 +4484,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B27">
         <v>4</v>
@@ -4410,7 +4492,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B28">
         <v>3</v>
@@ -4418,7 +4500,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4426,12 +4508,12 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B31">
         <v>0.03</v>
@@ -4439,12 +4521,12 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B33">
         <v>7</v>
@@ -4452,7 +4534,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B34">
         <v>4</v>
@@ -4460,7 +4542,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -4468,7 +4550,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B36">
         <v>3</v>
@@ -4476,7 +4558,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B37">
         <v>3</v>
@@ -4484,12 +4566,12 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B39">
         <v>0.03</v>
@@ -4497,20 +4579,20 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B41" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B42">
         <v>100</v>
@@ -4518,12 +4600,12 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B44">
         <v>20</v>
@@ -4531,12 +4613,12 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B46">
         <v>100</v>
@@ -4544,12 +4626,12 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B48">
         <v>50</v>
@@ -4557,12 +4639,12 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B50">
         <v>1.12516E-3</v>
@@ -4570,12 +4652,12 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B52">
         <v>2.3472099999999999E-4</v>
@@ -4583,25 +4665,25 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>200</v>
-      </c>
-      <c r="B54" s="58">
+        <v>198</v>
+      </c>
+      <c r="B54" s="37">
         <v>8.5876999999999995E-8</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B56">
         <v>10000</v>
@@ -4609,12 +4691,12 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B58">
         <v>2530</v>
@@ -4622,12 +4704,12 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B60">
         <v>3335</v>
@@ -4635,12 +4717,12 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B62">
         <v>-10</v>
@@ -4648,12 +4730,12 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B64">
         <v>80</v>
@@ -4661,12 +4743,12 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B66">
         <v>50</v>

</xml_diff>